<commit_message>
label font size change
</commit_message>
<xml_diff>
--- a/report/IPB1-2-LENR-COP.xlsx
+++ b/report/IPB1-2-LENR-COP.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="14385" yWindow="-15" windowWidth="14430" windowHeight="13860"/>
+    <workbookView xWindow="7920" yWindow="-195" windowWidth="12930" windowHeight="13860"/>
   </bookViews>
   <sheets>
     <sheet name="IPB2-LENR-COP" sheetId="5" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="52">
   <si>
     <t>NQ</t>
   </si>
@@ -276,7 +276,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -362,10 +362,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -415,13 +411,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -431,11 +425,52 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="22" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="26">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -939,86 +974,87 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BC79"/>
+  <dimension ref="A1:BC83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U15" sqref="U15:Y20"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Y89" sqref="Y89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="7" width="5.625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="5.625" style="49" customWidth="1"/>
+    <col min="8" max="8" width="5.625" style="47" customWidth="1"/>
     <col min="9" max="9" width="5.625" style="15" customWidth="1"/>
     <col min="10" max="12" width="5.625" style="1" customWidth="1"/>
     <col min="13" max="13" width="5.625" style="15" customWidth="1"/>
-    <col min="14" max="14" width="5.625" style="49" customWidth="1"/>
+    <col min="14" max="14" width="5.625" style="47" customWidth="1"/>
     <col min="15" max="40" width="5.625" style="1" customWidth="1"/>
     <col min="41" max="46" width="15.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="47" max="16384" width="9.125" style="1"/>
+    <col min="47" max="47" width="14.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="48" max="16384" width="9.125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:45" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="70" t="s">
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="66"/>
       <c r="L1" s="35"/>
       <c r="M1" s="18"/>
-      <c r="O1" s="69" t="s">
+      <c r="O1" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="P1" s="69"/>
-      <c r="Q1" s="69"/>
-      <c r="R1" s="69"/>
-      <c r="S1" s="69"/>
-      <c r="T1" s="69"/>
-      <c r="U1" s="69" t="s">
+      <c r="P1" s="65"/>
+      <c r="Q1" s="65"/>
+      <c r="R1" s="65"/>
+      <c r="S1" s="65"/>
+      <c r="T1" s="65"/>
+      <c r="U1" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="V1" s="69"/>
-      <c r="W1" s="69"/>
-      <c r="X1" s="69"/>
-      <c r="Y1" s="69"/>
-      <c r="Z1" s="69" t="s">
+      <c r="V1" s="65"/>
+      <c r="W1" s="65"/>
+      <c r="X1" s="65"/>
+      <c r="Y1" s="65"/>
+      <c r="Z1" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="AA1" s="69"/>
-      <c r="AB1" s="69"/>
-      <c r="AC1" s="69"/>
-      <c r="AD1" s="69"/>
-      <c r="AE1" s="69" t="s">
+      <c r="AA1" s="65"/>
+      <c r="AB1" s="65"/>
+      <c r="AC1" s="65"/>
+      <c r="AD1" s="65"/>
+      <c r="AE1" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="AF1" s="69"/>
-      <c r="AG1" s="69"/>
-      <c r="AH1" s="69"/>
-      <c r="AI1" s="69"/>
-      <c r="AJ1" s="69" t="s">
+      <c r="AF1" s="65"/>
+      <c r="AG1" s="65"/>
+      <c r="AH1" s="65"/>
+      <c r="AI1" s="65"/>
+      <c r="AJ1" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="AK1" s="69"/>
-      <c r="AL1" s="69"/>
-      <c r="AM1" s="69"/>
-      <c r="AN1" s="69"/>
-      <c r="AO1" s="69" t="s">
+      <c r="AK1" s="65"/>
+      <c r="AL1" s="65"/>
+      <c r="AM1" s="65"/>
+      <c r="AN1" s="65"/>
+      <c r="AO1" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="AP1" s="69"/>
-      <c r="AQ1" s="69"/>
-      <c r="AR1" s="69"/>
-      <c r="AS1" s="69"/>
+      <c r="AP1" s="65"/>
+      <c r="AQ1" s="65"/>
+      <c r="AR1" s="65"/>
+      <c r="AS1" s="65"/>
     </row>
     <row r="2" spans="1:45" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -1042,7 +1078,7 @@
       <c r="G2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="58" t="s">
+      <c r="H2" s="56" t="s">
         <v>12</v>
       </c>
       <c r="I2" s="16" t="s">
@@ -1199,7 +1235,7 @@
         <f>C3/(D3+E3)</f>
         <v>1.0664335664335665</v>
       </c>
-      <c r="H3" s="59"/>
+      <c r="H3" s="57"/>
       <c r="I3" s="16">
         <v>150</v>
       </c>
@@ -1213,7 +1249,7 @@
       </c>
       <c r="L3" s="37"/>
       <c r="M3" s="17"/>
-      <c r="N3" s="50" t="s">
+      <c r="N3" s="48" t="s">
         <v>25</v>
       </c>
       <c r="O3" s="2"/>
@@ -1242,7 +1278,7 @@
         <f>C4/(D4+E4)</f>
         <v>1.0702154626108997</v>
       </c>
-      <c r="H4" s="59"/>
+      <c r="H4" s="57"/>
       <c r="I4" s="16">
         <v>200</v>
       </c>
@@ -1254,7 +1290,7 @@
       </c>
       <c r="L4" s="37"/>
       <c r="M4" s="17"/>
-      <c r="N4" s="50"/>
+      <c r="N4" s="48"/>
       <c r="O4" s="2"/>
     </row>
     <row r="5" spans="1:45" x14ac:dyDescent="0.25">
@@ -1281,7 +1317,7 @@
         <f>C5/(D5+E5)</f>
         <v>1.0885978428351311</v>
       </c>
-      <c r="H5" s="59"/>
+      <c r="H5" s="57"/>
       <c r="I5" s="16">
         <v>250</v>
       </c>
@@ -1295,7 +1331,7 @@
       </c>
       <c r="L5" s="37"/>
       <c r="M5" s="17"/>
-      <c r="N5" s="50" t="s">
+      <c r="N5" s="48" t="s">
         <v>40</v>
       </c>
       <c r="O5" s="2" t="s">
@@ -1314,7 +1350,7 @@
       </c>
       <c r="L6" s="37"/>
       <c r="M6" s="17"/>
-      <c r="N6" s="51">
+      <c r="N6" s="49">
         <v>150</v>
       </c>
       <c r="O6" s="5">
@@ -1410,7 +1446,7 @@
       </c>
       <c r="L7" s="37"/>
       <c r="M7" s="17"/>
-      <c r="N7" s="51">
+      <c r="N7" s="49">
         <v>200</v>
       </c>
       <c r="O7" s="5">
@@ -1504,7 +1540,7 @@
       </c>
       <c r="L8" s="37"/>
       <c r="M8" s="17"/>
-      <c r="N8" s="51">
+      <c r="N8" s="49">
         <v>250</v>
       </c>
       <c r="O8" s="5">
@@ -1598,7 +1634,7 @@
         <v>-1.63987599095093E-2</v>
       </c>
       <c r="L9" s="37"/>
-      <c r="N9" s="51">
+      <c r="N9" s="49">
         <v>300</v>
       </c>
       <c r="O9" s="5">
@@ -1685,7 +1721,7 @@
       <c r="J10"/>
       <c r="K10"/>
       <c r="L10"/>
-      <c r="N10" s="51">
+      <c r="N10" s="49">
         <v>350</v>
       </c>
       <c r="O10" s="5">
@@ -1768,7 +1804,7 @@
       </c>
     </row>
     <row r="11" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="N11" s="51">
+      <c r="N11" s="49">
         <v>400</v>
       </c>
       <c r="O11" s="5">
@@ -1851,7 +1887,7 @@
       </c>
     </row>
     <row r="12" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="N12" s="50" t="s">
+      <c r="N12" s="48" t="s">
         <v>5</v>
       </c>
       <c r="O12" s="24"/>
@@ -1878,22 +1914,22 @@
       <c r="AN12" s="3"/>
     </row>
     <row r="13" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="C13" s="71" t="s">
+      <c r="C13" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="71"/>
-      <c r="E13" s="71"/>
-      <c r="F13" s="71"/>
-      <c r="G13" s="71"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="71" t="s">
+      <c r="D13" s="67"/>
+      <c r="E13" s="67"/>
+      <c r="F13" s="67"/>
+      <c r="G13" s="67"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="J13" s="71"/>
-      <c r="K13" s="71"/>
-      <c r="L13" s="71"/>
-      <c r="M13" s="71"/>
-      <c r="N13" s="50"/>
+      <c r="J13" s="67"/>
+      <c r="K13" s="67"/>
+      <c r="L13" s="67"/>
+      <c r="M13" s="67"/>
+      <c r="N13" s="48"/>
       <c r="O13" s="2"/>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
@@ -1939,7 +1975,7 @@
       <c r="G14" s="22">
         <v>300</v>
       </c>
-      <c r="H14" s="51"/>
+      <c r="H14" s="49"/>
       <c r="I14" s="16">
         <v>300</v>
       </c>
@@ -1955,7 +1991,7 @@
       <c r="M14" s="16">
         <v>300</v>
       </c>
-      <c r="N14" s="50" t="s">
+      <c r="N14" s="48" t="s">
         <v>40</v>
       </c>
       <c r="O14" s="2" t="s">
@@ -1990,10 +2026,10 @@
         <f t="shared" ref="G15:G20" si="13">T6-T15-(AD6-AD15)*$F$3-$G$3*(AI6+AN6-AI15-AN15)</f>
         <v>0.50109704794139143</v>
       </c>
-      <c r="H15" s="59"/>
+      <c r="H15" s="57"/>
       <c r="I15" s="16"/>
       <c r="M15" s="16"/>
-      <c r="N15" s="51">
+      <c r="N15" s="49">
         <v>150</v>
       </c>
       <c r="O15" s="11">
@@ -2103,10 +2139,10 @@
         <f t="shared" si="13"/>
         <v>2.0018245042521308</v>
       </c>
-      <c r="H16" s="59"/>
+      <c r="H16" s="57"/>
       <c r="I16" s="16"/>
       <c r="M16" s="16"/>
-      <c r="N16" s="51">
+      <c r="N16" s="49">
         <v>200</v>
       </c>
       <c r="O16" s="11">
@@ -2216,10 +2252,10 @@
         <f t="shared" si="13"/>
         <v>2.2527851759703541</v>
       </c>
-      <c r="H17" s="59"/>
+      <c r="H17" s="57"/>
       <c r="I17" s="16"/>
       <c r="M17" s="16"/>
-      <c r="N17" s="51">
+      <c r="N17" s="49">
         <v>250</v>
       </c>
       <c r="O17" s="11">
@@ -2329,10 +2365,10 @@
         <f t="shared" si="13"/>
         <v>3.3341612703247332</v>
       </c>
-      <c r="H18" s="59"/>
+      <c r="H18" s="57"/>
       <c r="I18" s="16"/>
       <c r="M18" s="16"/>
-      <c r="N18" s="51">
+      <c r="N18" s="49">
         <v>300</v>
       </c>
       <c r="O18" s="11">
@@ -2442,10 +2478,10 @@
         <f t="shared" si="13"/>
         <v>1.5916129949365159</v>
       </c>
-      <c r="H19" s="59"/>
+      <c r="H19" s="57"/>
       <c r="I19" s="16"/>
       <c r="M19" s="16"/>
-      <c r="N19" s="51">
+      <c r="N19" s="49">
         <v>350</v>
       </c>
       <c r="O19" s="11">
@@ -2555,10 +2591,10 @@
         <f t="shared" si="13"/>
         <v>2.0121469244486332</v>
       </c>
-      <c r="H20" s="59"/>
+      <c r="H20" s="57"/>
       <c r="I20" s="16"/>
       <c r="M20" s="16"/>
-      <c r="N20" s="51">
+      <c r="N20" s="49">
         <v>400</v>
       </c>
       <c r="O20" s="11">
@@ -2641,17 +2677,17 @@
       </c>
     </row>
     <row r="21" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="N21" s="50" t="s">
+      <c r="N21" s="48" t="s">
         <v>26</v>
       </c>
       <c r="O21" s="2"/>
     </row>
     <row r="22" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="N22" s="50"/>
+      <c r="N22" s="48"/>
       <c r="O22" s="2"/>
     </row>
     <row r="23" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="N23" s="50" t="s">
+      <c r="N23" s="48" t="s">
         <v>40</v>
       </c>
       <c r="O23" s="2" t="s">
@@ -2687,10 +2723,10 @@
         <f t="shared" ref="G24:G29" si="20">T6-T24-(AD6-AD24)*$F$3-$G$3*(AI6+AN6-AI24-AN24)</f>
         <v>-3.4184698029324654</v>
       </c>
-      <c r="H24" s="59"/>
+      <c r="H24" s="57"/>
       <c r="I24" s="16"/>
       <c r="M24" s="16"/>
-      <c r="N24" s="54">
+      <c r="N24" s="52">
         <v>150</v>
       </c>
       <c r="O24" s="11">
@@ -2787,10 +2823,10 @@
         <f t="shared" si="20"/>
         <v>-1.3924141365482727</v>
       </c>
-      <c r="H25" s="59"/>
+      <c r="H25" s="57"/>
       <c r="I25" s="16"/>
       <c r="M25" s="16"/>
-      <c r="N25" s="54">
+      <c r="N25" s="52">
         <v>200</v>
       </c>
       <c r="O25" s="11">
@@ -2887,10 +2923,10 @@
         <f t="shared" si="20"/>
         <v>0.64383618089404271</v>
       </c>
-      <c r="H26" s="59"/>
+      <c r="H26" s="57"/>
       <c r="I26" s="16"/>
       <c r="M26" s="16"/>
-      <c r="N26" s="54">
+      <c r="N26" s="52">
         <v>250</v>
       </c>
       <c r="O26" s="11">
@@ -2987,10 +3023,10 @@
         <f t="shared" si="20"/>
         <v>1.977392675722812</v>
       </c>
-      <c r="H27" s="59"/>
+      <c r="H27" s="57"/>
       <c r="I27" s="16"/>
       <c r="M27" s="16"/>
-      <c r="N27" s="54">
+      <c r="N27" s="52">
         <v>300</v>
       </c>
       <c r="O27" s="11">
@@ -3087,10 +3123,10 @@
         <f t="shared" si="20"/>
         <v>-1.9824035168627396</v>
       </c>
-      <c r="H28" s="59"/>
+      <c r="H28" s="57"/>
       <c r="I28" s="16"/>
       <c r="M28" s="16"/>
-      <c r="N28" s="54">
+      <c r="N28" s="52">
         <v>350</v>
       </c>
       <c r="O28" s="11">
@@ -3187,10 +3223,10 @@
         <f t="shared" si="20"/>
         <v>-2.1831677586301437</v>
       </c>
-      <c r="H29" s="59"/>
+      <c r="H29" s="57"/>
       <c r="I29" s="16"/>
       <c r="M29" s="16"/>
-      <c r="N29" s="54">
+      <c r="N29" s="52">
         <v>400</v>
       </c>
       <c r="O29" s="11">
@@ -3265,13 +3301,13 @@
       <c r="E30" s="12"/>
       <c r="F30" s="12"/>
       <c r="G30" s="12"/>
-      <c r="H30" s="59"/>
+      <c r="H30" s="57"/>
       <c r="I30" s="19"/>
       <c r="J30" s="19"/>
       <c r="K30" s="19"/>
       <c r="L30" s="19"/>
       <c r="M30" s="19"/>
-      <c r="N30" s="50" t="s">
+      <c r="N30" s="48" t="s">
         <v>43</v>
       </c>
       <c r="O30" s="37"/>
@@ -3308,13 +3344,13 @@
       <c r="E31" s="12"/>
       <c r="F31" s="12"/>
       <c r="G31" s="12"/>
-      <c r="H31" s="59"/>
+      <c r="H31" s="57"/>
       <c r="I31" s="19"/>
       <c r="J31" s="19"/>
       <c r="K31" s="19"/>
       <c r="L31" s="19"/>
       <c r="M31" s="19"/>
-      <c r="N31" s="63"/>
+      <c r="N31" s="61"/>
       <c r="O31" s="37"/>
       <c r="P31" s="39"/>
       <c r="Q31" s="39"/>
@@ -3349,30 +3385,30 @@
       <c r="E32" s="12"/>
       <c r="F32" s="12"/>
       <c r="G32" s="12"/>
-      <c r="H32" s="59"/>
+      <c r="H32" s="57"/>
       <c r="I32" s="19"/>
       <c r="J32" s="19"/>
       <c r="K32" s="19"/>
       <c r="L32" s="19"/>
       <c r="M32" s="19"/>
-      <c r="N32" s="63"/>
-      <c r="O32" s="41" t="s">
+      <c r="N32" s="61"/>
+      <c r="O32" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="P32" s="42"/>
-      <c r="Q32" s="42"/>
-      <c r="R32" s="42"/>
-      <c r="S32" s="42"/>
-      <c r="T32" s="42"/>
-      <c r="U32" s="42"/>
-      <c r="V32" s="42"/>
-      <c r="W32" s="42"/>
-      <c r="X32" s="42"/>
-      <c r="Y32" s="42"/>
-      <c r="Z32" s="42"/>
-      <c r="AA32" s="42"/>
-      <c r="AB32" s="42"/>
-      <c r="AC32" s="42"/>
+      <c r="P32" s="39"/>
+      <c r="Q32" s="39"/>
+      <c r="R32" s="39"/>
+      <c r="S32" s="39"/>
+      <c r="T32" s="39"/>
+      <c r="U32" s="39"/>
+      <c r="V32" s="39"/>
+      <c r="W32" s="39"/>
+      <c r="X32" s="39"/>
+      <c r="Y32" s="39"/>
+      <c r="Z32" s="39"/>
+      <c r="AA32" s="39"/>
+      <c r="AB32" s="39"/>
+      <c r="AC32" s="39"/>
       <c r="AD32" s="39"/>
       <c r="AE32" s="39"/>
       <c r="AF32" s="39"/>
@@ -3408,7 +3444,7 @@
         <v>0.76336346095317542</v>
       </c>
       <c r="G33" s="12"/>
-      <c r="H33" s="60">
+      <c r="H33" s="58">
         <v>1</v>
       </c>
       <c r="I33" s="19"/>
@@ -3425,7 +3461,7 @@
         <v>1.4011950937211404</v>
       </c>
       <c r="M33" s="19"/>
-      <c r="N33" s="56">
+      <c r="N33" s="54">
         <v>150</v>
       </c>
       <c r="O33" s="11">
@@ -3525,7 +3561,7 @@
         <v>-9.5958151596428953E-2</v>
       </c>
       <c r="G34" s="12"/>
-      <c r="H34" s="60">
+      <c r="H34" s="58">
         <v>1</v>
       </c>
       <c r="I34" s="19"/>
@@ -3542,7 +3578,7 @@
         <v>1.328286836864103</v>
       </c>
       <c r="M34" s="19"/>
-      <c r="N34" s="56">
+      <c r="N34" s="54">
         <v>200</v>
       </c>
       <c r="O34" s="11">
@@ -3642,7 +3678,7 @@
         <v>-0.60042622918877542</v>
       </c>
       <c r="G35" s="12"/>
-      <c r="H35" s="60">
+      <c r="H35" s="58">
         <v>1</v>
       </c>
       <c r="I35" s="19"/>
@@ -3659,7 +3695,7 @@
         <v>1.2833019251802766</v>
       </c>
       <c r="M35" s="19"/>
-      <c r="N35" s="56">
+      <c r="N35" s="54">
         <v>250</v>
       </c>
       <c r="O35" s="11">
@@ -3759,7 +3795,7 @@
         <v>-1.0339912983389998</v>
       </c>
       <c r="G36" s="12"/>
-      <c r="H36" s="60">
+      <c r="H36" s="58">
         <v>1</v>
       </c>
       <c r="I36" s="19"/>
@@ -3776,7 +3812,7 @@
         <v>1.3685938317163155</v>
       </c>
       <c r="M36" s="19"/>
-      <c r="N36" s="56">
+      <c r="N36" s="54">
         <v>300</v>
       </c>
       <c r="O36" s="11">
@@ -3860,13 +3896,13 @@
       <c r="E37" s="12"/>
       <c r="F37" s="12"/>
       <c r="G37" s="12"/>
-      <c r="H37" s="59"/>
+      <c r="H37" s="57"/>
       <c r="I37" s="19"/>
       <c r="J37" s="19"/>
       <c r="K37" s="19"/>
       <c r="L37" s="19"/>
       <c r="M37" s="19"/>
-      <c r="N37" s="56"/>
+      <c r="N37" s="54"/>
       <c r="O37"/>
       <c r="P37"/>
       <c r="Q37"/>
@@ -3901,13 +3937,13 @@
       <c r="E38" s="12"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12"/>
-      <c r="H38" s="59"/>
+      <c r="H38" s="57"/>
       <c r="I38" s="19"/>
       <c r="J38" s="19"/>
       <c r="K38" s="19"/>
       <c r="L38" s="19"/>
       <c r="M38" s="19"/>
-      <c r="N38" s="50" t="s">
+      <c r="N38" s="48" t="s">
         <v>42</v>
       </c>
       <c r="O38" s="37"/>
@@ -3944,13 +3980,13 @@
       <c r="E39" s="12"/>
       <c r="F39" s="12"/>
       <c r="G39" s="12"/>
-      <c r="H39" s="59"/>
+      <c r="H39" s="57"/>
       <c r="I39" s="19"/>
       <c r="J39" s="19"/>
       <c r="K39" s="19"/>
       <c r="L39" s="19"/>
       <c r="M39" s="19"/>
-      <c r="N39" s="63"/>
+      <c r="N39" s="61"/>
       <c r="O39" s="37"/>
       <c r="P39" s="39"/>
       <c r="Q39" s="39"/>
@@ -3985,30 +4021,30 @@
       <c r="E40" s="12"/>
       <c r="F40" s="12"/>
       <c r="G40" s="12"/>
-      <c r="H40" s="59"/>
+      <c r="H40" s="57"/>
       <c r="I40" s="19"/>
       <c r="J40" s="19"/>
       <c r="K40" s="19"/>
       <c r="L40" s="19"/>
       <c r="M40" s="19"/>
-      <c r="N40" s="63"/>
-      <c r="O40" s="41" t="s">
+      <c r="N40" s="61"/>
+      <c r="O40" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="P40" s="42"/>
-      <c r="Q40" s="42"/>
-      <c r="R40" s="42"/>
-      <c r="S40" s="42"/>
-      <c r="T40" s="42"/>
-      <c r="U40" s="42"/>
-      <c r="V40" s="42"/>
-      <c r="W40" s="42"/>
-      <c r="X40" s="42"/>
-      <c r="Y40" s="42"/>
-      <c r="Z40" s="42"/>
-      <c r="AA40" s="42"/>
-      <c r="AB40" s="42"/>
-      <c r="AC40" s="42"/>
+      <c r="P40" s="39"/>
+      <c r="Q40" s="39"/>
+      <c r="R40" s="39"/>
+      <c r="S40" s="39"/>
+      <c r="T40" s="39"/>
+      <c r="U40" s="39"/>
+      <c r="V40" s="39"/>
+      <c r="W40" s="39"/>
+      <c r="X40" s="39"/>
+      <c r="Y40" s="39"/>
+      <c r="Z40" s="39"/>
+      <c r="AA40" s="39"/>
+      <c r="AB40" s="39"/>
+      <c r="AC40" s="39"/>
       <c r="AD40" s="39"/>
       <c r="AE40" s="39"/>
       <c r="AF40" s="39"/>
@@ -4044,7 +4080,7 @@
         <v>1.068828922656806E-4</v>
       </c>
       <c r="G41" s="12"/>
-      <c r="H41" s="60">
+      <c r="H41" s="58">
         <v>1</v>
       </c>
       <c r="I41" s="19"/>
@@ -4061,7 +4097,7 @@
         <v>1.3092809170794484</v>
       </c>
       <c r="M41" s="19"/>
-      <c r="N41" s="56">
+      <c r="N41" s="54">
         <v>150</v>
       </c>
       <c r="O41" s="11">
@@ -4161,7 +4197,7 @@
         <v>-0.2333583917747058</v>
       </c>
       <c r="G42" s="12"/>
-      <c r="H42" s="60">
+      <c r="H42" s="58">
         <v>1</v>
       </c>
       <c r="I42" s="19"/>
@@ -4178,7 +4214,7 @@
         <v>1.415339047254744</v>
       </c>
       <c r="M42" s="19"/>
-      <c r="N42" s="56">
+      <c r="N42" s="54">
         <v>200</v>
       </c>
       <c r="O42" s="11">
@@ -4278,7 +4314,7 @@
         <v>-0.39428695778629108</v>
       </c>
       <c r="G43" s="12"/>
-      <c r="H43" s="60">
+      <c r="H43" s="58">
         <v>1</v>
       </c>
       <c r="I43" s="19"/>
@@ -4295,7 +4331,7 @@
         <v>1.3983845576963732</v>
       </c>
       <c r="M43" s="19"/>
-      <c r="N43" s="56">
+      <c r="N43" s="54">
         <v>250</v>
       </c>
       <c r="O43" s="11">
@@ -4379,13 +4415,13 @@
       <c r="E44" s="12"/>
       <c r="F44" s="12"/>
       <c r="G44" s="12"/>
-      <c r="H44" s="49"/>
+      <c r="H44" s="47"/>
       <c r="I44" s="19"/>
       <c r="J44" s="19"/>
       <c r="K44" s="19"/>
       <c r="L44" s="19"/>
       <c r="M44" s="19"/>
-      <c r="N44" s="55"/>
+      <c r="N44" s="53"/>
       <c r="O44"/>
       <c r="P44"/>
       <c r="Q44"/>
@@ -4435,13 +4471,13 @@
       <c r="E45" s="12"/>
       <c r="F45" s="12"/>
       <c r="G45" s="12"/>
-      <c r="H45" s="49"/>
+      <c r="H45" s="47"/>
       <c r="I45" s="19"/>
       <c r="J45" s="19"/>
       <c r="K45" s="19"/>
       <c r="L45" s="19"/>
       <c r="M45" s="19"/>
-      <c r="N45" s="56"/>
+      <c r="N45" s="54"/>
       <c r="O45"/>
       <c r="P45"/>
       <c r="Q45"/>
@@ -4475,7 +4511,7 @@
       <c r="K46" s="19"/>
       <c r="L46" s="19"/>
       <c r="M46" s="19"/>
-      <c r="N46" s="50" t="s">
+      <c r="N46" s="48" t="s">
         <v>29</v>
       </c>
       <c r="O46" s="2"/>
@@ -4486,7 +4522,7 @@
       <c r="K47" s="19"/>
       <c r="L47" s="19"/>
       <c r="M47" s="19"/>
-      <c r="N47" s="50"/>
+      <c r="N47" s="48"/>
       <c r="O47" s="2"/>
     </row>
     <row r="48" spans="1:55" x14ac:dyDescent="0.25">
@@ -4495,7 +4531,7 @@
       <c r="K48" s="19"/>
       <c r="L48" s="19"/>
       <c r="M48" s="19"/>
-      <c r="N48" s="50"/>
+      <c r="N48" s="48"/>
       <c r="O48" s="2" t="s">
         <v>27</v>
       </c>
@@ -4528,13 +4564,13 @@
         <f>T9-T49-(AD9-AD49)*$F$3-$G$3*(AI9+AN9-AI49-AN49)</f>
         <v>-1.1389783616152678</v>
       </c>
-      <c r="H49" s="59"/>
+      <c r="H49" s="57"/>
       <c r="I49" s="19"/>
       <c r="J49" s="19"/>
       <c r="K49" s="19"/>
       <c r="L49" s="19"/>
       <c r="M49" s="19"/>
-      <c r="N49" s="54">
+      <c r="N49" s="52">
         <v>300</v>
       </c>
       <c r="O49" s="11">
@@ -4639,13 +4675,13 @@
         <f>T9-T50-(AD9-AD50)*$F$3-$G$3*(AI9+AN9-AI50-AN50)</f>
         <v>-1.3191384478962687</v>
       </c>
-      <c r="H50" s="59"/>
+      <c r="H50" s="57"/>
       <c r="I50" s="19"/>
       <c r="J50" s="19"/>
       <c r="K50" s="19"/>
       <c r="L50" s="19"/>
       <c r="M50" s="19"/>
-      <c r="N50" s="51">
+      <c r="N50" s="49">
         <v>300</v>
       </c>
       <c r="O50" s="11">
@@ -4719,13 +4755,13 @@
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
-      <c r="H51" s="61"/>
+      <c r="H51" s="59"/>
       <c r="I51" s="19"/>
       <c r="J51" s="19"/>
       <c r="K51" s="19"/>
       <c r="L51" s="19"/>
       <c r="M51" s="19"/>
-      <c r="N51" s="50" t="s">
+      <c r="N51" s="48" t="s">
         <v>29</v>
       </c>
       <c r="O51" s="25"/>
@@ -4757,13 +4793,13 @@
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
-      <c r="H52" s="61"/>
+      <c r="H52" s="59"/>
       <c r="I52" s="19"/>
       <c r="J52" s="19"/>
       <c r="K52" s="19"/>
       <c r="L52" s="19"/>
       <c r="M52" s="19"/>
-      <c r="N52" s="50"/>
+      <c r="N52" s="48"/>
       <c r="O52" s="25"/>
       <c r="P52" s="4"/>
       <c r="Q52" s="4"/>
@@ -4793,13 +4829,13 @@
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
       <c r="G53" s="3"/>
-      <c r="H53" s="61"/>
+      <c r="H53" s="59"/>
       <c r="I53" s="19"/>
       <c r="J53" s="19"/>
       <c r="K53" s="19"/>
       <c r="L53" s="19"/>
       <c r="M53" s="19"/>
-      <c r="N53" s="50" t="s">
+      <c r="N53" s="48" t="s">
         <v>40</v>
       </c>
       <c r="O53" s="2" t="s">
@@ -4854,7 +4890,7 @@
         <f>T9-T54-(AD9-AD54)*$F$3-$G$3*(AI9+AN9-AI54-AN54)</f>
         <v>-1.6913816424623533</v>
       </c>
-      <c r="H54" s="60">
+      <c r="H54" s="58">
         <v>1.2</v>
       </c>
       <c r="I54" s="19">
@@ -4877,7 +4913,7 @@
         <f>(Y54*$H$54*$J$6+$K$6+$O54-T54)/(Y54*$H$54)</f>
         <v>1.1899907118243938</v>
       </c>
-      <c r="N54" s="56">
+      <c r="N54" s="54">
         <v>300</v>
       </c>
       <c r="O54" s="14">
@@ -4969,7 +5005,7 @@
       <c r="E55" s="12"/>
       <c r="F55" s="12"/>
       <c r="G55" s="12"/>
-      <c r="H55" s="60">
+      <c r="H55" s="58">
         <v>1.2</v>
       </c>
       <c r="I55" s="19">
@@ -4992,7 +5028,7 @@
         <f>(Y55*$H$55*$J$9+$K$9+$O55-T55)/(Y55*$H$55)</f>
         <v>1.093823460057433</v>
       </c>
-      <c r="N55" s="56">
+      <c r="N55" s="54">
         <v>600</v>
       </c>
       <c r="O55" s="14">
@@ -5075,13 +5111,13 @@
       </c>
     </row>
     <row r="56" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="H56" s="61"/>
+      <c r="H56" s="59"/>
       <c r="I56" s="19"/>
       <c r="J56" s="19"/>
       <c r="K56" s="19"/>
       <c r="L56" s="19"/>
       <c r="M56" s="19"/>
-      <c r="N56" s="50" t="s">
+      <c r="N56" s="48" t="s">
         <v>36</v>
       </c>
       <c r="O56" s="2"/>
@@ -5092,13 +5128,13 @@
       <c r="T56"/>
     </row>
     <row r="57" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="H57" s="61"/>
+      <c r="H57" s="59"/>
       <c r="I57" s="19"/>
       <c r="J57" s="19"/>
       <c r="K57" s="19"/>
       <c r="L57" s="19"/>
       <c r="M57" s="19"/>
-      <c r="N57" s="50"/>
+      <c r="N57" s="48"/>
       <c r="O57" s="2"/>
       <c r="P57"/>
       <c r="Q57"/>
@@ -5107,13 +5143,13 @@
       <c r="T57"/>
     </row>
     <row r="58" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="H58" s="61"/>
+      <c r="H58" s="59"/>
       <c r="I58" s="19"/>
       <c r="J58" s="19"/>
       <c r="K58" s="19"/>
       <c r="L58" s="19"/>
       <c r="M58" s="19"/>
-      <c r="N58" s="50"/>
+      <c r="N58" s="48"/>
       <c r="O58" s="2" t="s">
         <v>37</v>
       </c>
@@ -5152,7 +5188,7 @@
         <f t="shared" ref="G59:G64" si="30">T6-T59-(AD6-AD59)*$F$3-$G$3*(AI6+AN6-AI59-AN59)</f>
         <v>0.53212639110250626</v>
       </c>
-      <c r="H59" s="60">
+      <c r="H59" s="58">
         <v>1</v>
       </c>
       <c r="I59" s="19">
@@ -5175,7 +5211,7 @@
         <f>(Y59*$H$59*$J$3+$K$3+$O59-T59)/(Y59*$H$59)</f>
         <v>1.1698890545648439</v>
       </c>
-      <c r="N59" s="54">
+      <c r="N59" s="52">
         <v>150</v>
       </c>
       <c r="O59" s="27">
@@ -5304,7 +5340,7 @@
         <f t="shared" si="30"/>
         <v>1.8614282517427583E-2</v>
       </c>
-      <c r="H60" s="60">
+      <c r="H60" s="58">
         <v>1.06</v>
       </c>
       <c r="I60" s="19">
@@ -5327,7 +5363,7 @@
         <f>(Y60*$H$60*$J$4+$K$4+$O60-T60)/(Y60*$H$60)</f>
         <v>1.1967727309470368</v>
       </c>
-      <c r="N60" s="54">
+      <c r="N60" s="52">
         <v>200</v>
       </c>
       <c r="O60" s="27">
@@ -5456,7 +5492,7 @@
         <f t="shared" si="30"/>
         <v>-0.54729200545846801</v>
       </c>
-      <c r="H61" s="60">
+      <c r="H61" s="58">
         <v>1</v>
       </c>
       <c r="I61" s="19">
@@ -5479,7 +5515,7 @@
         <f>(Y61*$H$61*$J$5+$K$5+$O61-T61)/(Y61*$H$61)</f>
         <v>1.2374194883977547</v>
       </c>
-      <c r="N61" s="54">
+      <c r="N61" s="52">
         <v>250</v>
       </c>
       <c r="O61" s="27">
@@ -5579,155 +5615,155 @@
         <v>42630.141782407409</v>
       </c>
     </row>
-    <row r="62" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A62" s="23">
+    <row r="62" spans="1:46" s="75" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="68">
         <f t="shared" si="24"/>
         <v>300</v>
       </c>
-      <c r="B62" s="12">
+      <c r="B62" s="69">
         <f t="shared" si="25"/>
         <v>-1.4483726341463026</v>
       </c>
-      <c r="C62" s="12">
+      <c r="C62" s="69">
         <f t="shared" si="26"/>
         <v>-1.2989133749588582</v>
       </c>
-      <c r="D62" s="12">
+      <c r="D62" s="69">
         <f t="shared" si="27"/>
         <v>-2.3839796741687782</v>
       </c>
-      <c r="E62" s="12">
+      <c r="E62" s="69">
         <f t="shared" si="28"/>
         <v>-2.2946279974176207</v>
       </c>
-      <c r="F62" s="12">
+      <c r="F62" s="69">
         <f t="shared" si="29"/>
         <v>-2.2880774032027489</v>
       </c>
-      <c r="G62" s="12">
+      <c r="G62" s="69">
         <f t="shared" si="30"/>
         <v>-1.7543161972294024</v>
       </c>
-      <c r="H62" s="60">
-        <v>1.06</v>
-      </c>
-      <c r="I62" s="19">
+      <c r="H62" s="70">
+        <v>1.08</v>
+      </c>
+      <c r="I62" s="71">
         <f>(U62*$H$62*$J$6+$K$6+$O62-P62)/(U62*$H$62)</f>
-        <v>1.2930605526455645</v>
-      </c>
-      <c r="J62" s="19">
+        <v>1.2781177280533387</v>
+      </c>
+      <c r="J62" s="71">
         <f>(V62*$H$62*$J$6+$K$6+$O62-Q62)/(V62*$H$62)</f>
-        <v>1.2137181629357161</v>
-      </c>
-      <c r="K62" s="19">
+        <v>1.2002446418566355</v>
+      </c>
+      <c r="K62" s="71">
         <f>(W62*$H$62*$J$6+$K$6+$O62-R62)/(W62*$H$62)</f>
-        <v>1.2146242983440707</v>
-      </c>
-      <c r="L62" s="19">
+        <v>1.2011339969796504</v>
+      </c>
+      <c r="L62" s="71">
         <f>(X62*$H$62*$J$6+$K$6+$O62-S62)/(X62*$H$62)</f>
-        <v>1.2430628046558734</v>
-      </c>
-      <c r="M62" s="19">
+        <v>1.2290458642856787</v>
+      </c>
+      <c r="M62" s="71">
         <f>(Y62*$H$62*$J$6+$K$6+$O62-T62)/(Y62*$H$62)</f>
-        <v>1.2381915557846961</v>
-      </c>
-      <c r="N62" s="54">
+        <v>1.2242648237269311</v>
+      </c>
+      <c r="N62" s="72">
         <v>300</v>
       </c>
-      <c r="O62" s="27">
+      <c r="O62" s="73">
         <v>24.584489000000001</v>
       </c>
-      <c r="P62" s="27">
+      <c r="P62" s="73">
         <v>21.267337999999999</v>
       </c>
-      <c r="Q62" s="27">
+      <c r="Q62" s="73">
         <v>20.948191000000001</v>
       </c>
-      <c r="R62" s="27">
+      <c r="R62" s="73">
         <v>20.243701000000001</v>
       </c>
-      <c r="S62" s="27">
+      <c r="S62" s="73">
         <v>20.788577</v>
       </c>
-      <c r="T62" s="27">
+      <c r="T62" s="73">
         <v>21.490016000000001</v>
       </c>
-      <c r="U62" s="30">
+      <c r="U62" s="73">
         <v>3.9092684044117654</v>
       </c>
-      <c r="V62" s="30">
+      <c r="V62" s="73">
         <v>4.7493974044117646</v>
       </c>
-      <c r="W62" s="30">
+      <c r="W62" s="73">
         <v>5.6558230962962952</v>
       </c>
-      <c r="X62" s="30">
+      <c r="X62" s="73">
         <v>4.7642073676470602</v>
       </c>
-      <c r="Y62" s="30">
+      <c r="Y62" s="73">
         <v>3.9151511102941159</v>
       </c>
-      <c r="Z62" s="27">
+      <c r="Z62" s="73">
         <v>49.926560110294126</v>
       </c>
-      <c r="AA62" s="27">
+      <c r="AA62" s="73">
         <v>49.929095757352961</v>
       </c>
-      <c r="AB62" s="27">
+      <c r="AB62" s="73">
         <v>49.990274825925958</v>
       </c>
-      <c r="AC62" s="27">
+      <c r="AC62" s="73">
         <v>50.040242374999991</v>
       </c>
-      <c r="AD62" s="27">
+      <c r="AD62" s="73">
         <v>50.065050161764667</v>
       </c>
-      <c r="AE62" s="30">
+      <c r="AE62" s="73">
         <v>0.2820431911764707</v>
       </c>
-      <c r="AF62" s="30">
+      <c r="AF62" s="73">
         <v>0.53424416911764705</v>
       </c>
-      <c r="AG62" s="30">
+      <c r="AG62" s="73">
         <v>1.2621952481481482</v>
       </c>
-      <c r="AH62" s="30">
+      <c r="AH62" s="73">
         <v>0.63496296323529411</v>
       </c>
-      <c r="AI62" s="30">
+      <c r="AI62" s="73">
         <v>0.45394387499999983</v>
       </c>
-      <c r="AJ62" s="27">
+      <c r="AJ62" s="73">
         <v>31.329671051470587</v>
       </c>
-      <c r="AK62" s="27">
+      <c r="AK62" s="73">
         <v>28.521643242647059</v>
       </c>
-      <c r="AL62" s="27">
+      <c r="AL62" s="73">
         <v>27.431618037037062</v>
       </c>
-      <c r="AM62" s="27">
+      <c r="AM62" s="73">
         <v>28.634437683823521</v>
       </c>
-      <c r="AN62" s="27">
+      <c r="AN62" s="73">
         <v>31.563732904411754</v>
       </c>
-      <c r="AO62" s="31">
+      <c r="AO62" s="74">
         <v>42630.245972222219</v>
       </c>
-      <c r="AP62" s="31">
+      <c r="AP62" s="74">
         <v>42630.266805555555</v>
       </c>
-      <c r="AQ62" s="31">
+      <c r="AQ62" s="74">
         <v>42630.28765046296</v>
       </c>
-      <c r="AR62" s="31">
+      <c r="AR62" s="74">
         <v>42630.329328703701</v>
       </c>
-      <c r="AS62" s="31">
+      <c r="AS62" s="74">
         <v>42630.350162037037</v>
       </c>
-      <c r="AT62" s="31">
+      <c r="AT62" s="74">
         <v>42630.370995370373</v>
       </c>
     </row>
@@ -5760,7 +5796,7 @@
         <f t="shared" si="30"/>
         <v>-1.690970363964075</v>
       </c>
-      <c r="H63" s="60">
+      <c r="H63" s="58">
         <v>1</v>
       </c>
       <c r="I63" s="19">
@@ -5769,21 +5805,21 @@
       </c>
       <c r="J63" s="19">
         <f>(V63*$H$62*$J$6+$K$6+$O63-Q63)/(V63*$H$62)</f>
-        <v>1.1490370497664577</v>
+        <v>1.1367613270794001</v>
       </c>
       <c r="K63" s="19">
         <f>(W63*$H$62*$J$6+$K$6+$O63-R63)/(W63*$H$62)</f>
-        <v>1.1198559995574884</v>
+        <v>1.1081206666891155</v>
       </c>
       <c r="L63" s="19">
         <f>(X63*$H$62*$J$6+$K$6+$O63-S63)/(X63*$H$62)</f>
-        <v>1.1329296105113278</v>
+        <v>1.1209521737364017</v>
       </c>
       <c r="M63" s="19">
         <f>(Y63*$H$62*$J$6+$K$6+$O63-T63)/(Y63*$H$62)</f>
-        <v>1.148653576391796</v>
-      </c>
-      <c r="N63" s="54">
+        <v>1.1363849550635297</v>
+      </c>
+      <c r="N63" s="52">
         <v>350</v>
       </c>
       <c r="O63" s="27">
@@ -5912,7 +5948,7 @@
         <f t="shared" si="30"/>
         <v>-1.9809796140178664</v>
       </c>
-      <c r="H64" s="60">
+      <c r="H64" s="58">
         <v>1.06</v>
       </c>
       <c r="I64" s="19">
@@ -5935,7 +5971,7 @@
         <f>(Y64*$H$64*$J$8+$K$8+$O64-T64)/(Y64*$H$64)</f>
         <v>1.0521948750550463</v>
       </c>
-      <c r="N64" s="54">
+      <c r="N64" s="52">
         <v>400</v>
       </c>
       <c r="O64" s="27">
@@ -6035,730 +6071,874 @@
         <v>42630.829328703701</v>
       </c>
     </row>
-    <row r="65" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="H65" s="62"/>
-      <c r="J65" s="3"/>
-      <c r="N65" s="50" t="s">
+    <row r="65" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A65" s="64"/>
+      <c r="B65" s="12"/>
+      <c r="C65" s="12"/>
+      <c r="D65" s="12"/>
+      <c r="E65" s="12"/>
+      <c r="F65" s="12"/>
+      <c r="G65" s="12"/>
+      <c r="H65" s="58"/>
+      <c r="I65" s="19"/>
+      <c r="J65" s="19"/>
+      <c r="K65" s="19"/>
+      <c r="L65" s="19"/>
+      <c r="M65" s="19"/>
+      <c r="N65" s="48" t="s">
+        <v>36</v>
+      </c>
+      <c r="O65" s="2"/>
+      <c r="P65" s="76"/>
+      <c r="Q65" s="76"/>
+      <c r="R65" s="76"/>
+      <c r="S65" s="76"/>
+      <c r="T65" s="76"/>
+      <c r="U65" s="76"/>
+      <c r="V65" s="76"/>
+      <c r="W65" s="76"/>
+      <c r="X65" s="76"/>
+      <c r="Y65" s="76"/>
+      <c r="Z65" s="76"/>
+      <c r="AA65" s="76"/>
+      <c r="AB65" s="76"/>
+      <c r="AC65" s="76"/>
+      <c r="AD65" s="76"/>
+      <c r="AE65" s="76"/>
+      <c r="AF65" s="76"/>
+      <c r="AG65" s="76"/>
+      <c r="AH65" s="76"/>
+      <c r="AI65" s="76"/>
+      <c r="AJ65" s="76"/>
+      <c r="AK65" s="76"/>
+      <c r="AL65" s="76"/>
+      <c r="AM65" s="76"/>
+      <c r="AN65" s="76"/>
+      <c r="AO65" s="77"/>
+      <c r="AP65" s="77"/>
+      <c r="AQ65" s="77"/>
+      <c r="AR65" s="77"/>
+      <c r="AS65" s="77"/>
+      <c r="AT65" s="77"/>
+    </row>
+    <row r="66" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A66" s="64"/>
+      <c r="B66" s="12"/>
+      <c r="C66" s="12"/>
+      <c r="D66" s="12"/>
+      <c r="E66" s="12"/>
+      <c r="F66" s="12"/>
+      <c r="G66" s="12"/>
+      <c r="H66" s="58"/>
+      <c r="I66" s="19"/>
+      <c r="J66" s="19"/>
+      <c r="K66" s="19"/>
+      <c r="L66" s="19"/>
+      <c r="M66" s="19"/>
+      <c r="N66" s="48"/>
+      <c r="O66" s="2"/>
+      <c r="P66" s="76"/>
+      <c r="Q66" s="76"/>
+      <c r="R66" s="76"/>
+      <c r="S66" s="76"/>
+      <c r="T66" s="76"/>
+      <c r="U66" s="76"/>
+      <c r="V66" s="76"/>
+      <c r="W66" s="76"/>
+      <c r="X66" s="76"/>
+      <c r="Y66" s="76"/>
+      <c r="Z66" s="76"/>
+      <c r="AA66" s="76"/>
+      <c r="AB66" s="76"/>
+      <c r="AC66" s="76"/>
+      <c r="AD66" s="76"/>
+      <c r="AE66" s="76"/>
+      <c r="AF66" s="76"/>
+      <c r="AG66" s="76"/>
+      <c r="AH66" s="76"/>
+      <c r="AI66" s="76"/>
+      <c r="AJ66" s="76"/>
+      <c r="AK66" s="76"/>
+      <c r="AL66" s="76"/>
+      <c r="AM66" s="76"/>
+      <c r="AN66" s="76"/>
+      <c r="AO66" s="77"/>
+      <c r="AP66" s="77"/>
+      <c r="AQ66" s="77"/>
+      <c r="AR66" s="77"/>
+      <c r="AS66" s="77"/>
+      <c r="AT66" s="77"/>
+    </row>
+    <row r="67" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A67" s="64"/>
+      <c r="B67" s="12"/>
+      <c r="C67" s="12"/>
+      <c r="D67" s="12"/>
+      <c r="E67" s="12"/>
+      <c r="F67" s="12"/>
+      <c r="G67" s="12"/>
+      <c r="H67" s="58"/>
+      <c r="I67" s="19"/>
+      <c r="J67" s="19"/>
+      <c r="K67" s="19"/>
+      <c r="L67" s="19"/>
+      <c r="M67" s="19"/>
+      <c r="N67" s="48"/>
+      <c r="O67" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="P67" s="76"/>
+      <c r="Q67" s="76"/>
+      <c r="R67" s="76"/>
+      <c r="S67" s="76"/>
+      <c r="T67" s="76"/>
+      <c r="U67" s="76"/>
+      <c r="V67" s="76"/>
+      <c r="W67" s="76"/>
+      <c r="X67" s="76"/>
+      <c r="Y67" s="76"/>
+      <c r="Z67" s="76"/>
+      <c r="AA67" s="76"/>
+      <c r="AB67" s="76"/>
+      <c r="AC67" s="76"/>
+      <c r="AD67" s="76"/>
+      <c r="AE67" s="76"/>
+      <c r="AF67" s="76"/>
+      <c r="AG67" s="76"/>
+      <c r="AH67" s="76"/>
+      <c r="AI67" s="76"/>
+      <c r="AJ67" s="76"/>
+      <c r="AK67" s="76"/>
+      <c r="AL67" s="76"/>
+      <c r="AM67" s="76"/>
+      <c r="AN67" s="76"/>
+      <c r="AO67" s="77"/>
+      <c r="AP67" s="77"/>
+      <c r="AQ67" s="77"/>
+      <c r="AR67" s="77"/>
+      <c r="AS67" s="77"/>
+      <c r="AT67" s="77"/>
+    </row>
+    <row r="68" spans="1:47" s="75" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="68"/>
+      <c r="B68" s="69"/>
+      <c r="C68" s="69"/>
+      <c r="D68" s="69"/>
+      <c r="E68" s="69"/>
+      <c r="F68" s="69"/>
+      <c r="G68" s="69"/>
+      <c r="H68" s="70">
+        <v>1.08</v>
+      </c>
+      <c r="I68" s="71">
+        <f>(U68*$H$68*$J$6+$K$6+$O68-P68)/(U68*$H$68)</f>
+        <v>1.008818339245626</v>
+      </c>
+      <c r="J68" s="71">
+        <f t="shared" ref="J68:M68" si="31">(V68*$H$68*$J$6+$K$6+$O68-Q68)/(V68*$H$68)</f>
+        <v>1.004028026803965</v>
+      </c>
+      <c r="K68" s="71">
+        <f t="shared" si="31"/>
+        <v>0.993806051856991</v>
+      </c>
+      <c r="L68" s="71">
+        <f t="shared" si="31"/>
+        <v>1.0172986330905129</v>
+      </c>
+      <c r="M68" s="71">
+        <f t="shared" si="31"/>
+        <v>1.0508019925823737</v>
+      </c>
+      <c r="N68" s="72">
+        <v>600</v>
+      </c>
+      <c r="O68" s="73">
+        <v>74.032341902439001</v>
+      </c>
+      <c r="P68" s="73">
+        <v>71.060528512195106</v>
+      </c>
+      <c r="Q68" s="73">
+        <v>71.084728243902404</v>
+      </c>
+      <c r="R68" s="73">
+        <v>70.946126853658598</v>
+      </c>
+      <c r="S68" s="73">
+        <v>71.0234722195122</v>
+      </c>
+      <c r="T68" s="73">
+        <v>70.833931146341499</v>
+      </c>
+      <c r="U68" s="73">
+        <v>5.3116946097561</v>
+      </c>
+      <c r="V68" s="73">
+        <v>5.3175599024390303</v>
+      </c>
+      <c r="W68" s="73">
+        <v>5.6774292926829304</v>
+      </c>
+      <c r="X68" s="73">
+        <v>5.2914868780487803</v>
+      </c>
+      <c r="Y68" s="73">
+        <v>5.2883316829268301</v>
+      </c>
+      <c r="Z68" s="73">
+        <v>50.287989000000003</v>
+      </c>
+      <c r="AA68" s="73">
+        <v>50.295817902438998</v>
+      </c>
+      <c r="AB68" s="73">
+        <v>50.3355835121951</v>
+      </c>
+      <c r="AC68" s="73">
+        <v>50.348470390243897</v>
+      </c>
+      <c r="AD68" s="73">
+        <v>50.358690829268298</v>
+      </c>
+      <c r="AE68" s="73">
+        <v>0.48425858536585398</v>
+      </c>
+      <c r="AF68" s="73">
+        <v>0.782109146341464</v>
+      </c>
+      <c r="AG68" s="73">
+        <v>1.3459666097561001</v>
+      </c>
+      <c r="AH68" s="73">
+        <v>0.314033487804878</v>
+      </c>
+      <c r="AI68" s="73">
+        <v>0.21626400000000001</v>
+      </c>
+      <c r="AJ68" s="73">
+        <v>31.171222829268299</v>
+      </c>
+      <c r="AK68" s="73">
+        <v>28.840355146341501</v>
+      </c>
+      <c r="AL68" s="73">
+        <v>28.6199709268293</v>
+      </c>
+      <c r="AM68" s="73">
+        <v>28.685822048780501</v>
+      </c>
+      <c r="AN68" s="73">
+        <v>31.110990439024398</v>
+      </c>
+      <c r="AO68" s="74">
+        <v>42625.767060185186</v>
+      </c>
+      <c r="AP68" s="74">
+        <v>42625.780949074076</v>
+      </c>
+      <c r="AQ68" s="74">
+        <v>42625.822627314818</v>
+      </c>
+      <c r="AR68" s="74">
+        <v>42625.836527777778</v>
+      </c>
+      <c r="AS68" s="74">
+        <v>42625.850300925929</v>
+      </c>
+      <c r="AT68" s="74">
+        <v>42625.864189814813</v>
+      </c>
+      <c r="AU68" s="74"/>
+    </row>
+    <row r="69" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="H69" s="60"/>
+      <c r="J69" s="3"/>
+      <c r="N69" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="O65"/>
-      <c r="P65" s="5"/>
-      <c r="Q65" s="5"/>
-      <c r="R65" s="5"/>
-      <c r="S65" s="5"/>
-      <c r="T65" s="5"/>
-    </row>
-    <row r="66" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="N66" s="55"/>
-      <c r="O66"/>
-      <c r="P66" s="5"/>
-      <c r="Q66" s="5"/>
-      <c r="R66" s="5"/>
-      <c r="S66" s="5"/>
-      <c r="T66" s="5"/>
-    </row>
-    <row r="67" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="O67" s="2" t="s">
+      <c r="O69"/>
+      <c r="P69" s="5"/>
+      <c r="Q69" s="5"/>
+      <c r="R69" s="5"/>
+      <c r="S69" s="5"/>
+      <c r="T69" s="5"/>
+    </row>
+    <row r="70" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="N70" s="53"/>
+      <c r="O70"/>
+      <c r="P70" s="5"/>
+      <c r="Q70" s="5"/>
+      <c r="R70" s="5"/>
+      <c r="S70" s="5"/>
+      <c r="T70" s="5"/>
+    </row>
+    <row r="71" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="O71" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="68" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A68" s="43">
-        <f>N68</f>
+    <row r="72" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A72" s="41">
+        <f>N72</f>
         <v>250</v>
       </c>
-      <c r="B68" s="12">
-        <f>O8-O68</f>
+      <c r="B72" s="12">
+        <f>O8-O72</f>
         <v>-0.41817299999999946</v>
-      </c>
-      <c r="C68" s="12"/>
-      <c r="D68" s="12">
-        <f>Q8-Q68-(AA8-AA68)*$F$4-$G$4*(AF8+AK8-AF68-AK68)</f>
-        <v>7.5407298227453685</v>
-      </c>
-      <c r="E68" s="12">
-        <f>R8-R68-(AB8-AB68)*$F$5-$G$5*(AG8+AL8-AG68-AL68)</f>
-        <v>6.8546679891990614</v>
-      </c>
-      <c r="F68" s="12">
-        <f>S8-S68-(AC8-AC68)*$F$4-$G$4*(AH8+AM8-AH68-AM68)</f>
-        <v>7.3541682159359834</v>
-      </c>
-      <c r="G68" s="12"/>
-      <c r="H68" s="60">
-        <v>1</v>
-      </c>
-      <c r="I68" s="19"/>
-      <c r="J68" s="19">
-        <f t="shared" ref="J68:L69" si="31">(V68*$H68*$J$5+$K$5+$O68-Q68)/(V68*$H68)</f>
-        <v>1.3485912181115975</v>
-      </c>
-      <c r="K68" s="19">
-        <f t="shared" si="31"/>
-        <v>1.3285106960110227</v>
-      </c>
-      <c r="L68" s="19">
-        <f t="shared" si="31"/>
-        <v>1.3395762959682189</v>
-      </c>
-      <c r="M68" s="19"/>
-      <c r="N68" s="49">
-        <v>250</v>
-      </c>
-      <c r="O68" s="27">
-        <v>18.228331000000001</v>
-      </c>
-      <c r="P68" s="27"/>
-      <c r="Q68" s="27">
-        <v>14.562976870967701</v>
-      </c>
-      <c r="R68" s="27">
-        <v>13.9780723548387</v>
-      </c>
-      <c r="S68" s="27">
-        <v>14.6181962258065</v>
-      </c>
-      <c r="T68" s="27"/>
-      <c r="U68" s="30"/>
-      <c r="V68" s="30">
-        <v>4.2807538709677404</v>
-      </c>
-      <c r="W68" s="30">
-        <v>5.0771617741935504</v>
-      </c>
-      <c r="X68" s="30">
-        <v>4.2612692903225797</v>
-      </c>
-      <c r="Y68" s="30"/>
-      <c r="Z68" s="27"/>
-      <c r="AA68" s="27">
-        <v>50.269216096774201</v>
-      </c>
-      <c r="AB68" s="27">
-        <v>50.300657967741898</v>
-      </c>
-      <c r="AC68" s="27">
-        <v>50.310792612903199</v>
-      </c>
-      <c r="AD68" s="27"/>
-      <c r="AE68" s="30"/>
-      <c r="AF68" s="30">
-        <v>3.2489842580645201</v>
-      </c>
-      <c r="AG68" s="30">
-        <v>3.6162459354838701</v>
-      </c>
-      <c r="AH68" s="30">
-        <v>2.77801980645161</v>
-      </c>
-      <c r="AI68" s="30"/>
-      <c r="AJ68" s="27"/>
-      <c r="AK68" s="27">
-        <v>34.781154774193503</v>
-      </c>
-      <c r="AL68" s="27">
-        <v>32.837031838709699</v>
-      </c>
-      <c r="AM68" s="27">
-        <v>34.403320451612899</v>
-      </c>
-      <c r="AN68" s="27"/>
-      <c r="AO68" s="32"/>
-      <c r="AP68" s="32"/>
-      <c r="AQ68" s="32"/>
-      <c r="AR68" s="32"/>
-      <c r="AS68" s="32"/>
-      <c r="AT68" s="32"/>
-    </row>
-    <row r="69" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A69" s="43">
-        <f t="shared" ref="A69:A71" si="32">N69</f>
-        <v>275</v>
-      </c>
-      <c r="B69" s="12"/>
-      <c r="C69" s="12"/>
-      <c r="D69" s="12"/>
-      <c r="E69" s="12"/>
-      <c r="F69" s="12"/>
-      <c r="G69" s="12"/>
-      <c r="H69" s="60">
-        <v>1</v>
-      </c>
-      <c r="I69" s="19"/>
-      <c r="J69" s="19">
-        <f t="shared" si="31"/>
-        <v>1.3926462731039426</v>
-      </c>
-      <c r="K69" s="19">
-        <f t="shared" si="31"/>
-        <v>1.3470351899217541</v>
-      </c>
-      <c r="L69" s="19">
-        <f t="shared" si="31"/>
-        <v>1.3611709960268525</v>
-      </c>
-      <c r="M69" s="19"/>
-      <c r="N69" s="49">
-        <v>275</v>
-      </c>
-      <c r="O69" s="27">
-        <v>20.84873</v>
-      </c>
-      <c r="P69" s="27"/>
-      <c r="Q69" s="27">
-        <v>16.720784096774199</v>
-      </c>
-      <c r="R69" s="27">
-        <v>16.165159838709702</v>
-      </c>
-      <c r="S69" s="27">
-        <v>16.8826011612903</v>
-      </c>
-      <c r="T69" s="27"/>
-      <c r="U69" s="30"/>
-      <c r="V69" s="30">
-        <v>4.5830191290322597</v>
-      </c>
-      <c r="W69" s="30">
-        <v>5.4712432258064503</v>
-      </c>
-      <c r="X69" s="30">
-        <v>4.5629450645161302</v>
-      </c>
-      <c r="Y69" s="30"/>
-      <c r="Z69" s="27"/>
-      <c r="AA69" s="27">
-        <v>50.086105032258097</v>
-      </c>
-      <c r="AB69" s="27">
-        <v>50.136324354838699</v>
-      </c>
-      <c r="AC69" s="27">
-        <v>50.154668354838698</v>
-      </c>
-      <c r="AD69" s="27"/>
-      <c r="AE69" s="30"/>
-      <c r="AF69" s="30">
-        <v>2.5931445161290299</v>
-      </c>
-      <c r="AG69" s="30">
-        <v>3.1163965161290301</v>
-      </c>
-      <c r="AH69" s="30">
-        <v>2.5255309677419402</v>
-      </c>
-      <c r="AI69" s="30"/>
-      <c r="AJ69" s="27"/>
-      <c r="AK69" s="27">
-        <v>33.880331677419399</v>
-      </c>
-      <c r="AL69" s="27">
-        <v>32.070700483871001</v>
-      </c>
-      <c r="AM69" s="27">
-        <v>33.673540258064499</v>
-      </c>
-      <c r="AN69" s="27"/>
-    </row>
-    <row r="70" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A70" s="43">
-        <f t="shared" si="32"/>
-        <v>300</v>
-      </c>
-      <c r="B70" s="12">
-        <f>O9-O70</f>
-        <v>-0.62256263414630197</v>
-      </c>
-      <c r="C70" s="12"/>
-      <c r="D70" s="12">
-        <f>Q9-Q70-(AA9-AA70)*$F$4-$G$4*(AF9+AK9-AF70-AK70)</f>
-        <v>6.383730384368123</v>
-      </c>
-      <c r="E70" s="12">
-        <f>R9-R70-(AB9-AB70)*$F$4-$G$4*(AG9+AL9-AG70-AL70)</f>
-        <v>5.2704931315647032</v>
-      </c>
-      <c r="F70" s="12">
-        <f>S9-S70-(AC9-AC70)*$F$4-$G$4*(AH9+AM9-AH70-AM70)</f>
-        <v>5.5365936760857313</v>
-      </c>
-      <c r="G70" s="12"/>
-      <c r="H70" s="60">
-        <v>1</v>
-      </c>
-      <c r="I70" s="19"/>
-      <c r="J70" s="19">
-        <f t="shared" ref="J70:L71" si="33">(V70*$H70*$J$6+$K$6+$O70-Q70)/(V70*$H70)</f>
-        <v>1.4292088505581515</v>
-      </c>
-      <c r="K70" s="19">
-        <f t="shared" si="33"/>
-        <v>1.3996551684013179</v>
-      </c>
-      <c r="L70" s="19">
-        <f t="shared" si="33"/>
-        <v>1.3970758666353256</v>
-      </c>
-      <c r="M70" s="19"/>
-      <c r="N70" s="49">
-        <v>300</v>
-      </c>
-      <c r="O70" s="27">
-        <v>23.758679000000001</v>
-      </c>
-      <c r="P70" s="27"/>
-      <c r="Q70" s="27">
-        <v>19.245192258064499</v>
-      </c>
-      <c r="R70" s="27">
-        <v>18.4833052258065</v>
-      </c>
-      <c r="S70" s="27">
-        <v>19.404092806451601</v>
-      </c>
-      <c r="T70" s="27"/>
-      <c r="U70" s="30"/>
-      <c r="V70" s="30">
-        <v>4.8141535806451596</v>
-      </c>
-      <c r="W70" s="30">
-        <v>5.8039247096774202</v>
-      </c>
-      <c r="X70" s="30">
-        <v>4.8095347419354804</v>
-      </c>
-      <c r="Y70" s="30"/>
-      <c r="Z70" s="27"/>
-      <c r="AA70" s="27">
-        <v>49.887546516128999</v>
-      </c>
-      <c r="AB70" s="27">
-        <v>49.931536322580598</v>
-      </c>
-      <c r="AC70" s="27">
-        <v>49.955233387096797</v>
-      </c>
-      <c r="AD70" s="27"/>
-      <c r="AE70" s="30"/>
-      <c r="AF70" s="30">
-        <v>2.3391682903225801</v>
-      </c>
-      <c r="AG70" s="30">
-        <v>2.7492468387096798</v>
-      </c>
-      <c r="AH70" s="30">
-        <v>2.1072768387096801</v>
-      </c>
-      <c r="AI70" s="30"/>
-      <c r="AJ70" s="27"/>
-      <c r="AK70" s="27">
-        <v>33.354199903225798</v>
-      </c>
-      <c r="AL70" s="27">
-        <v>31.4189674516129</v>
-      </c>
-      <c r="AM70" s="27">
-        <v>33.253998548387102</v>
-      </c>
-      <c r="AN70" s="27"/>
-    </row>
-    <row r="71" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A71" s="43">
-        <f t="shared" si="32"/>
-        <v>325</v>
-      </c>
-      <c r="B71" s="12"/>
-      <c r="C71" s="12"/>
-      <c r="D71" s="12"/>
-      <c r="E71" s="12"/>
-      <c r="F71" s="12"/>
-      <c r="G71" s="12"/>
-      <c r="H71" s="60">
-        <v>1</v>
-      </c>
-      <c r="I71" s="19"/>
-      <c r="J71" s="19">
-        <f t="shared" si="33"/>
-        <v>1.404791706237438</v>
-      </c>
-      <c r="K71" s="19">
-        <f t="shared" si="33"/>
-        <v>1.4032432581090277</v>
-      </c>
-      <c r="L71" s="19">
-        <f t="shared" si="33"/>
-        <v>1.3999544650678855</v>
-      </c>
-      <c r="M71" s="19"/>
-      <c r="N71" s="49">
-        <v>325</v>
-      </c>
-      <c r="O71" s="27">
-        <v>26.714182000000001</v>
-      </c>
-      <c r="P71" s="27"/>
-      <c r="Q71" s="27">
-        <v>22.238615580645199</v>
-      </c>
-      <c r="R71" s="27">
-        <v>21.284031258064498</v>
-      </c>
-      <c r="S71" s="27">
-        <v>22.263480032258101</v>
-      </c>
-      <c r="T71" s="27"/>
-      <c r="U71" s="30"/>
-      <c r="V71" s="30">
-        <v>4.9008330645161298</v>
-      </c>
-      <c r="W71" s="30">
-        <v>5.9499858387096802</v>
-      </c>
-      <c r="X71" s="30">
-        <v>4.8995659032258096</v>
-      </c>
-      <c r="Y71" s="30"/>
-      <c r="Z71" s="27"/>
-      <c r="AA71" s="27">
-        <v>49.632656096774198</v>
-      </c>
-      <c r="AB71" s="27">
-        <v>49.700629967741897</v>
-      </c>
-      <c r="AC71" s="27">
-        <v>49.734550645161299</v>
-      </c>
-      <c r="AD71" s="27"/>
-      <c r="AE71" s="30"/>
-      <c r="AF71" s="30">
-        <v>2.4207534838709699</v>
-      </c>
-      <c r="AG71" s="30">
-        <v>4.0216372580645201</v>
-      </c>
-      <c r="AH71" s="30">
-        <v>3.6216999677419399</v>
-      </c>
-      <c r="AI71" s="30"/>
-      <c r="AJ71" s="27"/>
-      <c r="AK71" s="27">
-        <v>33.475266741935499</v>
-      </c>
-      <c r="AL71" s="27">
-        <v>32.1663261935484</v>
-      </c>
-      <c r="AM71" s="27">
-        <v>34.252079000000002</v>
-      </c>
-      <c r="AN71" s="27"/>
-    </row>
-    <row r="72" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A72" s="43">
-        <f>N72</f>
-        <v>400</v>
-      </c>
-      <c r="B72" s="12">
-        <f>O11-O72</f>
-        <v>-0.87733897560969609</v>
       </c>
       <c r="C72" s="12"/>
       <c r="D72" s="12">
-        <f>Q11-Q72-(AA11-AA72)*$F$4-$G$4*(AF11+AK11-AF72-AK72)</f>
-        <v>9.0962728536279762</v>
+        <f>Q8-Q72-(AA8-AA72)*$F$4-$G$4*(AF8+AK8-AF72-AK72)</f>
+        <v>7.5407298227453685</v>
       </c>
       <c r="E72" s="12">
-        <f>R11-R72-(AB11-AB72)*$F$4-$G$4*(AG11+AL11-AG72-AL72)</f>
-        <v>7.9803121383120121</v>
+        <f>R8-R72-(AB8-AB72)*$F$5-$G$5*(AG8+AL8-AG72-AL72)</f>
+        <v>6.8546679891990614</v>
       </c>
       <c r="F72" s="12">
-        <f>S11-S72-(AC11-AC72)*$F$4-$G$4*(AH11+AM11-AH72-AM72)</f>
-        <v>9.1121737730832777</v>
+        <f>S8-S72-(AC8-AC72)*$F$4-$G$4*(AH8+AM8-AH72-AM72)</f>
+        <v>7.3541682159359834</v>
       </c>
       <c r="G72" s="12"/>
-      <c r="H72" s="60">
+      <c r="H72" s="58">
         <v>1</v>
       </c>
       <c r="I72" s="19"/>
       <c r="J72" s="19">
-        <f>(V72*$H72*$J$8+$K$8+$O72-Q72)/(V72*$H72)</f>
-        <v>1.0629715744014709</v>
+        <f t="shared" ref="J72:L73" si="32">(V72*$H72*$J$5+$K$5+$O72-Q72)/(V72*$H72)</f>
+        <v>1.3485912181115975</v>
       </c>
       <c r="K72" s="19">
-        <f>(W72*$H72*$J$8+$K$8+$O72-R72)/(W72*$H72)</f>
-        <v>1.0243987804504953</v>
+        <f t="shared" si="32"/>
+        <v>1.3285106960110227</v>
       </c>
       <c r="L72" s="19">
-        <f>(X72*$H72*$J$8+$K$8+$O72-S72)/(X72*$H72)</f>
-        <v>1.1030434792735895</v>
+        <f t="shared" si="32"/>
+        <v>1.3395762959682189</v>
       </c>
       <c r="M72" s="19"/>
-      <c r="N72" s="49">
-        <v>400</v>
+      <c r="N72" s="47">
+        <v>250</v>
       </c>
       <c r="O72" s="27">
-        <v>36.130347999999998</v>
+        <v>18.228331000000001</v>
       </c>
       <c r="P72" s="27"/>
       <c r="Q72" s="27">
-        <v>33.610354225806503</v>
+        <v>14.562976870967701</v>
       </c>
       <c r="R72" s="27">
-        <v>33.476327096774199</v>
+        <v>13.9780723548387</v>
       </c>
       <c r="S72" s="27">
-        <v>33.439099290322602</v>
+        <v>14.6181962258065</v>
       </c>
       <c r="T72" s="27"/>
       <c r="U72" s="30"/>
       <c r="V72" s="30">
-        <v>4.0154207419354799</v>
+        <v>4.2807538709677404</v>
       </c>
       <c r="W72" s="30">
-        <v>4.5013699677419403</v>
+        <v>5.0771617741935504</v>
       </c>
       <c r="X72" s="30">
-        <v>4.0307946451612899</v>
+        <v>4.2612692903225797</v>
       </c>
       <c r="Y72" s="30"/>
       <c r="Z72" s="27"/>
       <c r="AA72" s="27">
-        <v>50.4111786774194</v>
+        <v>50.269216096774201</v>
       </c>
       <c r="AB72" s="27">
-        <v>49.813302774193602</v>
+        <v>50.300657967741898</v>
       </c>
       <c r="AC72" s="27">
-        <v>49.478309000000003</v>
+        <v>50.310792612903199</v>
       </c>
       <c r="AD72" s="27"/>
       <c r="AE72" s="30"/>
       <c r="AF72" s="30">
-        <v>5.2934330645161296</v>
+        <v>3.2489842580645201</v>
       </c>
       <c r="AG72" s="30">
-        <v>6.0988026129032296</v>
+        <v>3.6162459354838701</v>
       </c>
       <c r="AH72" s="30">
-        <v>5.5709035806451599</v>
+        <v>2.77801980645161</v>
       </c>
       <c r="AI72" s="30"/>
       <c r="AJ72" s="27"/>
       <c r="AK72" s="27">
-        <v>36.272245677419399</v>
+        <v>34.781154774193503</v>
       </c>
       <c r="AL72" s="27">
-        <v>35.2183322580645</v>
+        <v>32.837031838709699</v>
       </c>
       <c r="AM72" s="27">
-        <v>36.6170531290323</v>
+        <v>34.403320451612899</v>
       </c>
       <c r="AN72" s="27"/>
-    </row>
-    <row r="73" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A73" s="43"/>
+      <c r="AO72" s="32"/>
+      <c r="AP72" s="32"/>
+      <c r="AQ72" s="32"/>
+      <c r="AR72" s="32"/>
+      <c r="AS72" s="32"/>
+      <c r="AT72" s="32"/>
+    </row>
+    <row r="73" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A73" s="41">
+        <f t="shared" ref="A73:A75" si="33">N73</f>
+        <v>275</v>
+      </c>
       <c r="B73" s="12"/>
       <c r="C73" s="12"/>
       <c r="D73" s="12"/>
       <c r="E73" s="12"/>
       <c r="F73" s="12"/>
       <c r="G73" s="12"/>
-    </row>
-    <row r="74" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A74" s="64">
-        <f>N74</f>
-        <v>250</v>
-      </c>
-      <c r="D74" s="67">
-        <f>AF74+AK74-Q74</f>
-        <v>7.1674476365989666</v>
-      </c>
-      <c r="E74" s="67">
-        <f t="shared" ref="E74:F76" si="34">AG74+AL74-R74</f>
-        <v>5.9992259712217839</v>
-      </c>
-      <c r="F74" s="67">
+      <c r="H73" s="58">
+        <v>1</v>
+      </c>
+      <c r="I73" s="19"/>
+      <c r="J73" s="19">
+        <f t="shared" si="32"/>
+        <v>1.3926462731039426</v>
+      </c>
+      <c r="K73" s="19">
+        <f t="shared" si="32"/>
+        <v>1.3470351899217541</v>
+      </c>
+      <c r="L73" s="19">
+        <f t="shared" si="32"/>
+        <v>1.3611709960268525</v>
+      </c>
+      <c r="M73" s="19"/>
+      <c r="N73" s="47">
+        <v>275</v>
+      </c>
+      <c r="O73" s="27">
+        <v>20.84873</v>
+      </c>
+      <c r="P73" s="27"/>
+      <c r="Q73" s="27">
+        <v>16.720784096774199</v>
+      </c>
+      <c r="R73" s="27">
+        <v>16.165159838709702</v>
+      </c>
+      <c r="S73" s="27">
+        <v>16.8826011612903</v>
+      </c>
+      <c r="T73" s="27"/>
+      <c r="U73" s="30"/>
+      <c r="V73" s="30">
+        <v>4.5830191290322597</v>
+      </c>
+      <c r="W73" s="30">
+        <v>5.4712432258064503</v>
+      </c>
+      <c r="X73" s="30">
+        <v>4.5629450645161302</v>
+      </c>
+      <c r="Y73" s="30"/>
+      <c r="Z73" s="27"/>
+      <c r="AA73" s="27">
+        <v>50.086105032258097</v>
+      </c>
+      <c r="AB73" s="27">
+        <v>50.136324354838699</v>
+      </c>
+      <c r="AC73" s="27">
+        <v>50.154668354838698</v>
+      </c>
+      <c r="AD73" s="27"/>
+      <c r="AE73" s="30"/>
+      <c r="AF73" s="30">
+        <v>2.5931445161290299</v>
+      </c>
+      <c r="AG73" s="30">
+        <v>3.1163965161290301</v>
+      </c>
+      <c r="AH73" s="30">
+        <v>2.5255309677419402</v>
+      </c>
+      <c r="AI73" s="30"/>
+      <c r="AJ73" s="27"/>
+      <c r="AK73" s="27">
+        <v>33.880331677419399</v>
+      </c>
+      <c r="AL73" s="27">
+        <v>32.070700483871001</v>
+      </c>
+      <c r="AM73" s="27">
+        <v>33.673540258064499</v>
+      </c>
+      <c r="AN73" s="27"/>
+    </row>
+    <row r="74" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A74" s="41">
+        <f t="shared" si="33"/>
+        <v>300</v>
+      </c>
+      <c r="B74" s="12">
+        <f>O9-O74</f>
+        <v>-0.62256263414630197</v>
+      </c>
+      <c r="C74" s="12"/>
+      <c r="D74" s="12">
+        <f>Q9-Q74-(AA9-AA74)*$F$4-$G$4*(AF9+AK9-AF74-AK74)</f>
+        <v>6.383730384368123</v>
+      </c>
+      <c r="E74" s="12">
+        <f>R9-R74-(AB9-AB74)*$F$4-$G$4*(AG9+AL9-AG74-AL74)</f>
+        <v>5.2704931315647032</v>
+      </c>
+      <c r="F74" s="12">
+        <f>S9-S74-(AC9-AC74)*$F$4-$G$4*(AH9+AM9-AH74-AM74)</f>
+        <v>5.5365936760857313</v>
+      </c>
+      <c r="G74" s="12"/>
+      <c r="H74" s="58">
+        <v>1</v>
+      </c>
+      <c r="I74" s="19"/>
+      <c r="J74" s="19">
+        <f t="shared" ref="J74:L75" si="34">(V74*$H74*$J$6+$K$6+$O74-Q74)/(V74*$H74)</f>
+        <v>1.4292088505581515</v>
+      </c>
+      <c r="K74" s="19">
         <f t="shared" si="34"/>
-        <v>6.2338838163592021</v>
-      </c>
-      <c r="N74" s="49">
-        <v>250</v>
-      </c>
-      <c r="O74" s="3">
-        <f>O68-O8</f>
-        <v>0.41817299999999946</v>
-      </c>
-      <c r="Q74" s="3">
-        <f t="shared" ref="Q74:S74" si="35">Q68-Q8</f>
-        <v>1.3558528709677002</v>
-      </c>
-      <c r="R74" s="3">
-        <f>R68-R8</f>
-        <v>0.73277830605819894</v>
-      </c>
-      <c r="S74" s="3">
-        <f t="shared" si="35"/>
-        <v>1.3959997380015992</v>
-      </c>
-      <c r="AF74" s="3">
-        <f t="shared" ref="AF74" si="36">AF68-AF8</f>
-        <v>1.5411549432497051</v>
-      </c>
-      <c r="AG74" s="3">
-        <f>AG68-AG8</f>
-        <v>1.2051048181999198</v>
-      </c>
-      <c r="AH74" s="3">
-        <f t="shared" ref="AH74" si="37">AH68-AH8</f>
-        <v>1.1715657694145731</v>
-      </c>
-      <c r="AK74" s="3">
-        <f t="shared" ref="AK74" si="38">AK68-AK8</f>
-        <v>6.9821455643169621</v>
-      </c>
-      <c r="AL74" s="3">
-        <f>AL68-AL8</f>
-        <v>5.5268994590800631</v>
-      </c>
-      <c r="AM74" s="3">
-        <f t="shared" ref="AM74" si="39">AM68-AM8</f>
-        <v>6.4583177849462281</v>
-      </c>
-    </row>
-    <row r="75" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A75" s="64">
-        <f t="shared" ref="A75:A76" si="40">N75</f>
+        <v>1.3996551684013179</v>
+      </c>
+      <c r="L74" s="19">
+        <f t="shared" si="34"/>
+        <v>1.3970758666353256</v>
+      </c>
+      <c r="M74" s="19"/>
+      <c r="N74" s="47">
         <v>300</v>
       </c>
-      <c r="D75" s="67">
-        <f t="shared" ref="D75" si="41">AF75+AK75-Q75</f>
-        <v>6.2271425780613958</v>
-      </c>
-      <c r="E75" s="67">
+      <c r="O74" s="27">
+        <v>23.758679000000001</v>
+      </c>
+      <c r="P74" s="27"/>
+      <c r="Q74" s="27">
+        <v>19.245192258064499</v>
+      </c>
+      <c r="R74" s="27">
+        <v>18.4833052258065</v>
+      </c>
+      <c r="S74" s="27">
+        <v>19.404092806451601</v>
+      </c>
+      <c r="T74" s="27"/>
+      <c r="U74" s="30"/>
+      <c r="V74" s="30">
+        <v>4.8141535806451596</v>
+      </c>
+      <c r="W74" s="30">
+        <v>5.8039247096774202</v>
+      </c>
+      <c r="X74" s="30">
+        <v>4.8095347419354804</v>
+      </c>
+      <c r="Y74" s="30"/>
+      <c r="Z74" s="27"/>
+      <c r="AA74" s="27">
+        <v>49.887546516128999</v>
+      </c>
+      <c r="AB74" s="27">
+        <v>49.931536322580598</v>
+      </c>
+      <c r="AC74" s="27">
+        <v>49.955233387096797</v>
+      </c>
+      <c r="AD74" s="27"/>
+      <c r="AE74" s="30"/>
+      <c r="AF74" s="30">
+        <v>2.3391682903225801</v>
+      </c>
+      <c r="AG74" s="30">
+        <v>2.7492468387096798</v>
+      </c>
+      <c r="AH74" s="30">
+        <v>2.1072768387096801</v>
+      </c>
+      <c r="AI74" s="30"/>
+      <c r="AJ74" s="27"/>
+      <c r="AK74" s="27">
+        <v>33.354199903225798</v>
+      </c>
+      <c r="AL74" s="27">
+        <v>31.4189674516129</v>
+      </c>
+      <c r="AM74" s="27">
+        <v>33.253998548387102</v>
+      </c>
+      <c r="AN74" s="27"/>
+    </row>
+    <row r="75" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A75" s="41">
+        <f t="shared" si="33"/>
+        <v>325</v>
+      </c>
+      <c r="B75" s="12"/>
+      <c r="C75" s="12"/>
+      <c r="D75" s="12"/>
+      <c r="E75" s="12"/>
+      <c r="F75" s="12"/>
+      <c r="G75" s="12"/>
+      <c r="H75" s="58">
+        <v>1</v>
+      </c>
+      <c r="I75" s="19"/>
+      <c r="J75" s="19">
         <f t="shared" si="34"/>
-        <v>5.2917002557988759</v>
-      </c>
-      <c r="F75" s="67">
+        <v>1.404791706237438</v>
+      </c>
+      <c r="K75" s="19">
         <f t="shared" si="34"/>
-        <v>5.540275122048417</v>
-      </c>
-      <c r="N75" s="49">
-        <v>300</v>
-      </c>
-      <c r="O75" s="65">
-        <f>O70-O9</f>
-        <v>0.62256263414630197</v>
-      </c>
-      <c r="P75" s="66"/>
-      <c r="Q75" s="65">
-        <f>Q70-Q9</f>
-        <v>0.60416830684500056</v>
-      </c>
-      <c r="R75" s="65">
-        <f>R70-R9</f>
-        <v>-0.16192653029110105</v>
-      </c>
-      <c r="S75" s="65">
-        <f t="shared" ref="S75" si="42">S70-S9</f>
-        <v>0.70388866011010265</v>
-      </c>
-      <c r="AF75" s="65">
-        <f>AF70-AF9</f>
-        <v>1.0240663520509752</v>
-      </c>
-      <c r="AG75" s="65">
-        <f>AG70-AG9</f>
-        <v>0.70630548685782912</v>
-      </c>
-      <c r="AH75" s="65">
-        <f t="shared" ref="AH75" si="43">AH70-AH9</f>
-        <v>0.8028488016726425</v>
-      </c>
-      <c r="AK75" s="65">
-        <f>AK70-AK9</f>
-        <v>5.807244532855421</v>
-      </c>
-      <c r="AL75" s="65">
-        <f>AL70-AL9</f>
-        <v>4.4234682386499458</v>
-      </c>
-      <c r="AM75" s="65">
-        <f t="shared" ref="AM75" si="44">AM70-AM9</f>
-        <v>5.4413149804858776</v>
-      </c>
-    </row>
-    <row r="76" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A76" s="64">
-        <f t="shared" si="40"/>
+        <v>1.4032432581090277</v>
+      </c>
+      <c r="L75" s="19">
+        <f t="shared" si="34"/>
+        <v>1.3999544650678855</v>
+      </c>
+      <c r="M75" s="19"/>
+      <c r="N75" s="47">
+        <v>325</v>
+      </c>
+      <c r="O75" s="27">
+        <v>26.714182000000001</v>
+      </c>
+      <c r="P75" s="27"/>
+      <c r="Q75" s="27">
+        <v>22.238615580645199</v>
+      </c>
+      <c r="R75" s="27">
+        <v>21.284031258064498</v>
+      </c>
+      <c r="S75" s="27">
+        <v>22.263480032258101</v>
+      </c>
+      <c r="T75" s="27"/>
+      <c r="U75" s="30"/>
+      <c r="V75" s="30">
+        <v>4.9008330645161298</v>
+      </c>
+      <c r="W75" s="30">
+        <v>5.9499858387096802</v>
+      </c>
+      <c r="X75" s="30">
+        <v>4.8995659032258096</v>
+      </c>
+      <c r="Y75" s="30"/>
+      <c r="Z75" s="27"/>
+      <c r="AA75" s="27">
+        <v>49.632656096774198</v>
+      </c>
+      <c r="AB75" s="27">
+        <v>49.700629967741897</v>
+      </c>
+      <c r="AC75" s="27">
+        <v>49.734550645161299</v>
+      </c>
+      <c r="AD75" s="27"/>
+      <c r="AE75" s="30"/>
+      <c r="AF75" s="30">
+        <v>2.4207534838709699</v>
+      </c>
+      <c r="AG75" s="30">
+        <v>4.0216372580645201</v>
+      </c>
+      <c r="AH75" s="30">
+        <v>3.6216999677419399</v>
+      </c>
+      <c r="AI75" s="30"/>
+      <c r="AJ75" s="27"/>
+      <c r="AK75" s="27">
+        <v>33.475266741935499</v>
+      </c>
+      <c r="AL75" s="27">
+        <v>32.1663261935484</v>
+      </c>
+      <c r="AM75" s="27">
+        <v>34.252079000000002</v>
+      </c>
+      <c r="AN75" s="27"/>
+    </row>
+    <row r="76" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A76" s="41">
+        <f>N76</f>
         <v>400</v>
       </c>
-      <c r="D76" s="67">
-        <f>AF76+AK76-Q76</f>
-        <v>7.3023148946294771</v>
-      </c>
-      <c r="E76" s="67">
-        <f t="shared" si="34"/>
-        <v>6.9096528364150949</v>
-      </c>
-      <c r="F76" s="67">
-        <f t="shared" si="34"/>
-        <v>8.3536862623238584</v>
-      </c>
-      <c r="N76" s="49">
+      <c r="B76" s="12">
+        <f>O11-O76</f>
+        <v>-0.87733897560969609</v>
+      </c>
+      <c r="C76" s="12"/>
+      <c r="D76" s="12">
+        <f>Q11-Q76-(AA11-AA76)*$F$4-$G$4*(AF11+AK11-AF76-AK76)</f>
+        <v>9.0962728536279762</v>
+      </c>
+      <c r="E76" s="12">
+        <f>R11-R76-(AB11-AB76)*$F$4-$G$4*(AG11+AL11-AG76-AL76)</f>
+        <v>7.9803121383120121</v>
+      </c>
+      <c r="F76" s="12">
+        <f>S11-S76-(AC11-AC76)*$F$4-$G$4*(AH11+AM11-AH76-AM76)</f>
+        <v>9.1121737730832777</v>
+      </c>
+      <c r="G76" s="12"/>
+      <c r="H76" s="58">
+        <v>1</v>
+      </c>
+      <c r="I76" s="19"/>
+      <c r="J76" s="19">
+        <f>(V76*$H76*$J$8+$K$8+$O76-Q76)/(V76*$H76)</f>
+        <v>1.0629715744014709</v>
+      </c>
+      <c r="K76" s="19">
+        <f>(W76*$H76*$J$8+$K$8+$O76-R76)/(W76*$H76)</f>
+        <v>1.0243987804504953</v>
+      </c>
+      <c r="L76" s="19">
+        <f>(X76*$H76*$J$8+$K$8+$O76-S76)/(X76*$H76)</f>
+        <v>1.1030434792735895</v>
+      </c>
+      <c r="M76" s="19"/>
+      <c r="N76" s="47">
         <v>400</v>
       </c>
-      <c r="O76" s="3">
-        <f>O72-O11</f>
-        <v>0.87733897560969609</v>
-      </c>
-      <c r="Q76" s="3">
-        <f t="shared" ref="Q76:S76" si="45">Q72-Q11</f>
-        <v>2.9789938843431045</v>
-      </c>
-      <c r="R76" s="3">
-        <f t="shared" si="45"/>
-        <v>2.7879503162863983</v>
-      </c>
-      <c r="S76" s="3">
-        <f t="shared" si="45"/>
-        <v>2.7771920708104005</v>
-      </c>
-      <c r="AF76" s="3">
-        <f t="shared" ref="AF76:AH76" si="46">AF72-AF11</f>
-        <v>3.1603837743926717</v>
-      </c>
-      <c r="AG76" s="3">
-        <f t="shared" si="46"/>
-        <v>3.3515343094976582</v>
-      </c>
-      <c r="AH76" s="3">
-        <f t="shared" si="46"/>
-        <v>3.7310038213859009</v>
-      </c>
-      <c r="AK76" s="3">
-        <f>AK72-AK11</f>
-        <v>7.1209250045799095</v>
-      </c>
-      <c r="AL76" s="3">
-        <f t="shared" ref="AL76:AM76" si="47">AL72-AL11</f>
-        <v>6.3460688432038346</v>
-      </c>
-      <c r="AM76" s="3">
-        <f t="shared" si="47"/>
-        <v>7.399874511748358</v>
-      </c>
-    </row>
-    <row r="77" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A77" s="68" t="s">
+      <c r="O76" s="27">
+        <v>36.130347999999998</v>
+      </c>
+      <c r="P76" s="27"/>
+      <c r="Q76" s="27">
+        <v>33.610354225806503</v>
+      </c>
+      <c r="R76" s="27">
+        <v>33.476327096774199</v>
+      </c>
+      <c r="S76" s="27">
+        <v>33.439099290322602</v>
+      </c>
+      <c r="T76" s="27"/>
+      <c r="U76" s="30"/>
+      <c r="V76" s="30">
+        <v>4.0154207419354799</v>
+      </c>
+      <c r="W76" s="30">
+        <v>4.5013699677419403</v>
+      </c>
+      <c r="X76" s="30">
+        <v>4.0307946451612899</v>
+      </c>
+      <c r="Y76" s="30"/>
+      <c r="Z76" s="27"/>
+      <c r="AA76" s="27">
+        <v>50.4111786774194</v>
+      </c>
+      <c r="AB76" s="27">
+        <v>49.813302774193602</v>
+      </c>
+      <c r="AC76" s="27">
+        <v>49.478309000000003</v>
+      </c>
+      <c r="AD76" s="27"/>
+      <c r="AE76" s="30"/>
+      <c r="AF76" s="30">
+        <v>5.2934330645161296</v>
+      </c>
+      <c r="AG76" s="30">
+        <v>6.0988026129032296</v>
+      </c>
+      <c r="AH76" s="30">
+        <v>5.5709035806451599</v>
+      </c>
+      <c r="AI76" s="30"/>
+      <c r="AJ76" s="27"/>
+      <c r="AK76" s="27">
+        <v>36.272245677419399</v>
+      </c>
+      <c r="AL76" s="27">
+        <v>35.2183322580645</v>
+      </c>
+      <c r="AM76" s="27">
+        <v>36.6170531290323</v>
+      </c>
+      <c r="AN76" s="27"/>
+    </row>
+    <row r="77" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A77" s="41"/>
+      <c r="B77" s="12"/>
+      <c r="C77" s="12"/>
+      <c r="D77" s="12"/>
+      <c r="E77" s="12"/>
+      <c r="F77" s="12"/>
+      <c r="G77" s="12"/>
+    </row>
+    <row r="78" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A78" s="64"/>
+      <c r="D78" s="62"/>
+      <c r="E78" s="62"/>
+      <c r="F78" s="62"/>
+      <c r="O78" s="3"/>
+      <c r="Q78" s="3"/>
+      <c r="R78" s="3"/>
+      <c r="S78" s="3"/>
+      <c r="AF78" s="3"/>
+      <c r="AG78" s="3"/>
+      <c r="AH78" s="3"/>
+      <c r="AK78" s="3"/>
+      <c r="AL78" s="3"/>
+      <c r="AM78" s="3"/>
+    </row>
+    <row r="79" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A79" s="64"/>
+      <c r="D79" s="62"/>
+      <c r="E79" s="62"/>
+      <c r="F79" s="62"/>
+      <c r="O79" s="3"/>
+      <c r="Q79" s="3"/>
+      <c r="R79" s="3"/>
+      <c r="S79" s="3"/>
+      <c r="AF79" s="3"/>
+      <c r="AG79" s="3"/>
+      <c r="AH79" s="3"/>
+      <c r="AK79" s="3"/>
+      <c r="AL79" s="3"/>
+      <c r="AM79" s="3"/>
+    </row>
+    <row r="80" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A80" s="64"/>
+      <c r="D80" s="62"/>
+      <c r="E80" s="62"/>
+      <c r="F80" s="62"/>
+      <c r="O80" s="3"/>
+      <c r="Q80" s="3"/>
+      <c r="R80" s="3"/>
+      <c r="S80" s="3"/>
+      <c r="AF80" s="3"/>
+      <c r="AG80" s="3"/>
+      <c r="AH80" s="3"/>
+      <c r="AK80" s="3"/>
+      <c r="AL80" s="3"/>
+      <c r="AM80" s="3"/>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="63" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="78" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="79" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
         <v>50</v>
       </c>
     </row>
@@ -6776,72 +6956,77 @@
     <mergeCell ref="I1:K1"/>
   </mergeCells>
   <conditionalFormatting sqref="C15:G20">
-    <cfRule type="cellIs" dxfId="22" priority="53" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="54" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="54" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="55" operator="greaterThan">
       <formula>3.19</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24:G29">
-    <cfRule type="cellIs" dxfId="20" priority="51" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="52" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="52" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="22" priority="53" operator="greaterThan">
       <formula>3.19</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54:G54">
-    <cfRule type="cellIs" dxfId="18" priority="47" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="48" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="48" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="20" priority="49" operator="greaterThan">
       <formula>3.19</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C73">
-    <cfRule type="cellIs" dxfId="16" priority="19" operator="greaterThan">
+  <conditionalFormatting sqref="C77">
+    <cfRule type="cellIs" dxfId="19" priority="20" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="20" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="21" operator="greaterThan">
       <formula>3.19</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D73:G73">
-    <cfRule type="cellIs" dxfId="14" priority="17" operator="greaterThan">
+  <conditionalFormatting sqref="D77:G77">
+    <cfRule type="cellIs" dxfId="17" priority="18" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="19" operator="greaterThan">
       <formula>3.19</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B33:B36">
-    <cfRule type="cellIs" dxfId="12" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="8" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I33:M36">
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="6" operator="greaterThan">
       <formula>1.3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I41:M43">
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="5" operator="greaterThan">
       <formula>1.3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I54:M55">
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="greaterThan">
       <formula>1.3</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I59:M64">
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="greaterThan">
+  <conditionalFormatting sqref="I59:M67">
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="greaterThan">
       <formula>1.3</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I68:M72">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="greaterThan">
+  <conditionalFormatting sqref="I72:M76">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="greaterThan">
+      <formula>1.3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I68:M68">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
       <formula>1.3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6861,11 +7046,11 @@
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="7" width="5.625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="5.625" style="47" customWidth="1"/>
+    <col min="8" max="8" width="5.625" style="45" customWidth="1"/>
     <col min="9" max="9" width="5.625" style="15" customWidth="1"/>
     <col min="10" max="12" width="5.625" style="1" customWidth="1"/>
     <col min="13" max="13" width="5.625" style="15" customWidth="1"/>
-    <col min="14" max="14" width="5.625" style="49" customWidth="1"/>
+    <col min="14" max="14" width="5.625" style="47" customWidth="1"/>
     <col min="15" max="40" width="5.625" style="1" customWidth="1"/>
     <col min="41" max="41" width="14.375" style="1" bestFit="1" customWidth="1"/>
     <col min="42" max="45" width="15.125" style="1" bestFit="1" customWidth="1"/>
@@ -6874,31 +7059,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:46" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="70" t="s">
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="66"/>
+      <c r="L1" s="66"/>
       <c r="M1" s="18"/>
-      <c r="O1" s="69" t="s">
+      <c r="O1" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="P1" s="69"/>
-      <c r="Q1" s="69"/>
-      <c r="R1" s="69"/>
-      <c r="S1" s="69"/>
-      <c r="T1" s="69"/>
+      <c r="P1" s="65"/>
+      <c r="Q1" s="65"/>
+      <c r="R1" s="65"/>
+      <c r="S1" s="65"/>
+      <c r="T1" s="65"/>
       <c r="U1" s="7" t="s">
         <v>39</v>
       </c>
@@ -6906,35 +7091,35 @@
       <c r="W1" s="7"/>
       <c r="X1" s="7"/>
       <c r="Y1" s="7"/>
-      <c r="Z1" s="69" t="s">
+      <c r="Z1" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="AA1" s="69"/>
-      <c r="AB1" s="69"/>
-      <c r="AC1" s="69"/>
-      <c r="AD1" s="69"/>
-      <c r="AE1" s="69" t="s">
+      <c r="AA1" s="65"/>
+      <c r="AB1" s="65"/>
+      <c r="AC1" s="65"/>
+      <c r="AD1" s="65"/>
+      <c r="AE1" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="AF1" s="69"/>
-      <c r="AG1" s="69"/>
-      <c r="AH1" s="69"/>
-      <c r="AI1" s="69"/>
-      <c r="AJ1" s="69" t="s">
+      <c r="AF1" s="65"/>
+      <c r="AG1" s="65"/>
+      <c r="AH1" s="65"/>
+      <c r="AI1" s="65"/>
+      <c r="AJ1" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="AK1" s="69"/>
-      <c r="AL1" s="69"/>
-      <c r="AM1" s="69"/>
-      <c r="AN1" s="69"/>
-      <c r="AO1" s="69" t="s">
+      <c r="AK1" s="65"/>
+      <c r="AL1" s="65"/>
+      <c r="AM1" s="65"/>
+      <c r="AN1" s="65"/>
+      <c r="AO1" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="AP1" s="69"/>
-      <c r="AQ1" s="69"/>
-      <c r="AR1" s="69"/>
-      <c r="AS1" s="69"/>
-      <c r="AT1" s="69"/>
+      <c r="AP1" s="65"/>
+      <c r="AQ1" s="65"/>
+      <c r="AR1" s="65"/>
+      <c r="AS1" s="65"/>
+      <c r="AT1" s="65"/>
     </row>
     <row r="2" spans="1:46" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -6958,7 +7143,7 @@
       <c r="G2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="45" t="s">
+      <c r="H2" s="43" t="s">
         <v>12</v>
       </c>
       <c r="I2" s="16" t="s">
@@ -7118,7 +7303,7 @@
         <f>C3/(D3+E3)</f>
         <v>1.1434730538922155</v>
       </c>
-      <c r="H3" s="46"/>
+      <c r="H3" s="44"/>
       <c r="I3" s="16">
         <v>150</v>
       </c>
@@ -7132,7 +7317,7 @@
       </c>
       <c r="L3" s="17"/>
       <c r="M3" s="17"/>
-      <c r="N3" s="50" t="s">
+      <c r="N3" s="48" t="s">
         <v>24</v>
       </c>
     </row>
@@ -7160,7 +7345,7 @@
         <f>C4/(D4+E4)</f>
         <v>1.1467404378157326</v>
       </c>
-      <c r="H4" s="46"/>
+      <c r="H4" s="44"/>
       <c r="I4" s="16">
         <v>200</v>
       </c>
@@ -7172,7 +7357,7 @@
       </c>
       <c r="L4" s="17"/>
       <c r="M4" s="17"/>
-      <c r="N4" s="50"/>
+      <c r="N4" s="48"/>
     </row>
     <row r="5" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -7198,7 +7383,7 @@
         <f>C5/(D5+E5)</f>
         <v>1.1654411764705883</v>
       </c>
-      <c r="H5" s="46"/>
+      <c r="H5" s="44"/>
       <c r="I5" s="16">
         <v>250</v>
       </c>
@@ -7212,7 +7397,7 @@
       </c>
       <c r="L5" s="17"/>
       <c r="M5" s="17"/>
-      <c r="N5" s="50"/>
+      <c r="N5" s="48"/>
       <c r="O5" s="2" t="s">
         <v>33</v>
       </c>
@@ -7229,7 +7414,7 @@
       </c>
       <c r="L6" s="17"/>
       <c r="M6" s="17"/>
-      <c r="N6" s="51">
+      <c r="N6" s="49">
         <v>150</v>
       </c>
       <c r="O6" s="26">
@@ -7311,7 +7496,7 @@
       </c>
       <c r="L7" s="17"/>
       <c r="M7" s="17"/>
-      <c r="N7" s="51">
+      <c r="N7" s="49">
         <v>200</v>
       </c>
       <c r="O7" s="26">
@@ -7391,7 +7576,7 @@
       </c>
       <c r="L8" s="17"/>
       <c r="M8" s="17"/>
-      <c r="N8" s="51">
+      <c r="N8" s="49">
         <v>250</v>
       </c>
       <c r="O8" s="26">
@@ -7471,7 +7656,7 @@
         <v>-1.63987599095093E-2</v>
       </c>
       <c r="L9" s="17"/>
-      <c r="N9" s="51">
+      <c r="N9" s="49">
         <v>300</v>
       </c>
       <c r="O9" s="26">
@@ -7540,7 +7725,7 @@
       <c r="AO9" s="3"/>
     </row>
     <row r="10" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="N10" s="51">
+      <c r="N10" s="49">
         <v>350</v>
       </c>
       <c r="O10" s="26">
@@ -7609,7 +7794,7 @@
       <c r="AO10" s="3"/>
     </row>
     <row r="11" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="N11" s="51">
+      <c r="N11" s="49">
         <v>400</v>
       </c>
       <c r="O11" s="26">
@@ -7678,21 +7863,21 @@
       <c r="AO11" s="3"/>
     </row>
     <row r="12" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="C12" s="71" t="s">
+      <c r="C12" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="71"/>
-      <c r="E12" s="71"/>
-      <c r="F12" s="71"/>
-      <c r="G12" s="71"/>
-      <c r="I12" s="71" t="s">
+      <c r="D12" s="67"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="67"/>
+      <c r="G12" s="67"/>
+      <c r="I12" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="J12" s="71"/>
-      <c r="K12" s="71"/>
-      <c r="L12" s="71"/>
-      <c r="M12" s="71"/>
-      <c r="N12" s="52" t="s">
+      <c r="J12" s="67"/>
+      <c r="K12" s="67"/>
+      <c r="L12" s="67"/>
+      <c r="M12" s="67"/>
+      <c r="N12" s="50" t="s">
         <v>5</v>
       </c>
       <c r="O12" s="3"/>
@@ -7755,7 +7940,7 @@
       <c r="M13" s="16">
         <v>300</v>
       </c>
-      <c r="N13" s="51"/>
+      <c r="N13" s="49"/>
     </row>
     <row r="14" spans="1:46" x14ac:dyDescent="0.25">
       <c r="C14" s="34"/>
@@ -7768,7 +7953,7 @@
       <c r="K14" s="34"/>
       <c r="L14" s="34"/>
       <c r="M14" s="16"/>
-      <c r="N14" s="53"/>
+      <c r="N14" s="51"/>
       <c r="O14" s="2" t="s">
         <v>34</v>
       </c>
@@ -7801,10 +7986,10 @@
         <f t="shared" ref="G15:G20" si="5">T6-T15-(AD6-AD15)*$F$3-$G$3*(AI6+AN6-AI15-AN15)</f>
         <v>-1.2142054011014094</v>
       </c>
-      <c r="H15" s="46"/>
+      <c r="H15" s="44"/>
       <c r="I15" s="16"/>
       <c r="M15" s="16"/>
-      <c r="N15" s="51">
+      <c r="N15" s="49">
         <v>150</v>
       </c>
       <c r="O15" s="26">
@@ -7900,10 +8085,10 @@
         <f t="shared" si="5"/>
         <v>-0.56889870508180707</v>
       </c>
-      <c r="H16" s="46"/>
+      <c r="H16" s="44"/>
       <c r="I16" s="16"/>
       <c r="M16" s="16"/>
-      <c r="N16" s="51">
+      <c r="N16" s="49">
         <v>200</v>
       </c>
       <c r="O16" s="26">
@@ -7999,10 +8184,10 @@
         <f t="shared" si="5"/>
         <v>-1.0671519792638884</v>
       </c>
-      <c r="H17" s="46"/>
+      <c r="H17" s="44"/>
       <c r="I17" s="16"/>
       <c r="M17" s="16"/>
-      <c r="N17" s="51">
+      <c r="N17" s="49">
         <v>250</v>
       </c>
       <c r="O17" s="26">
@@ -8098,10 +8283,10 @@
         <f t="shared" si="5"/>
         <v>0.34138990693689775</v>
       </c>
-      <c r="H18" s="46"/>
+      <c r="H18" s="44"/>
       <c r="I18" s="16"/>
       <c r="M18" s="16"/>
-      <c r="N18" s="51">
+      <c r="N18" s="49">
         <v>300</v>
       </c>
       <c r="O18" s="26">
@@ -8197,10 +8382,10 @@
         <f t="shared" si="5"/>
         <v>-1.0531913820662506</v>
       </c>
-      <c r="H19" s="46"/>
+      <c r="H19" s="44"/>
       <c r="I19" s="16"/>
       <c r="M19" s="16"/>
-      <c r="N19" s="51">
+      <c r="N19" s="49">
         <v>350</v>
       </c>
       <c r="O19" s="26">
@@ -8296,10 +8481,10 @@
         <f t="shared" si="5"/>
         <v>-3.6122474310283801</v>
       </c>
-      <c r="H20" s="46"/>
+      <c r="H20" s="44"/>
       <c r="I20" s="16"/>
       <c r="M20" s="16"/>
-      <c r="N20" s="51">
+      <c r="N20" s="49">
         <v>400</v>
       </c>
       <c r="O20" s="26">
@@ -8368,15 +8553,15 @@
       <c r="AO20" s="3"/>
     </row>
     <row r="21" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="N21" s="52" t="s">
+      <c r="N21" s="50" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="N22" s="53"/>
+      <c r="N22" s="51"/>
     </row>
     <row r="23" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="N23" s="53"/>
+      <c r="N23" s="51"/>
       <c r="O23" s="2" t="s">
         <v>35</v>
       </c>
@@ -8410,10 +8595,10 @@
         <f t="shared" ref="G24:G29" si="12">T6-T24-(AD6-AD24)*$F$3-$G$3*(AI6+AN6-AI24-AN24)</f>
         <v>-2.2091838044552516</v>
       </c>
-      <c r="H24" s="46"/>
+      <c r="H24" s="44"/>
       <c r="I24" s="16"/>
       <c r="M24" s="16"/>
-      <c r="N24" s="54">
+      <c r="N24" s="52">
         <v>150</v>
       </c>
       <c r="O24" s="26">
@@ -8510,10 +8695,10 @@
         <f t="shared" si="12"/>
         <v>-1.8629536076591575</v>
       </c>
-      <c r="H25" s="46"/>
+      <c r="H25" s="44"/>
       <c r="I25" s="16"/>
       <c r="M25" s="16"/>
-      <c r="N25" s="54">
+      <c r="N25" s="52">
         <v>200</v>
       </c>
       <c r="O25" s="26">
@@ -8610,10 +8795,10 @@
         <f t="shared" si="12"/>
         <v>-1.7253601607741622</v>
       </c>
-      <c r="H26" s="46"/>
+      <c r="H26" s="44"/>
       <c r="I26" s="16"/>
       <c r="M26" s="16"/>
-      <c r="N26" s="54">
+      <c r="N26" s="52">
         <v>250</v>
       </c>
       <c r="O26" s="26">
@@ -8710,10 +8895,10 @@
         <f t="shared" si="12"/>
         <v>-0.56849139505752477</v>
       </c>
-      <c r="H27" s="46"/>
+      <c r="H27" s="44"/>
       <c r="I27" s="16"/>
       <c r="M27" s="16"/>
-      <c r="N27" s="54">
+      <c r="N27" s="52">
         <v>300</v>
       </c>
       <c r="O27" s="26">
@@ -8810,10 +8995,10 @@
         <f t="shared" si="12"/>
         <v>-2.256729754594355</v>
       </c>
-      <c r="H28" s="46"/>
+      <c r="H28" s="44"/>
       <c r="I28" s="16"/>
       <c r="M28" s="16"/>
-      <c r="N28" s="54">
+      <c r="N28" s="52">
         <v>350</v>
       </c>
       <c r="O28" s="26">
@@ -8910,10 +9095,10 @@
         <f t="shared" si="12"/>
         <v>-3.0653317871144354</v>
       </c>
-      <c r="H29" s="46"/>
+      <c r="H29" s="44"/>
       <c r="I29" s="16"/>
       <c r="M29" s="16"/>
-      <c r="N29" s="54">
+      <c r="N29" s="52">
         <v>400</v>
       </c>
       <c r="O29" s="26">
@@ -8982,7 +9167,7 @@
       <c r="AO29" s="3"/>
     </row>
     <row r="30" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="N30" s="50" t="s">
+      <c r="N30" s="48" t="s">
         <v>47</v>
       </c>
       <c r="O30"/>
@@ -8997,7 +9182,7 @@
         <f>O34-Q34</f>
         <v>4.4644832258064007</v>
       </c>
-      <c r="N31" s="55"/>
+      <c r="N31" s="53"/>
       <c r="O31"/>
       <c r="P31" s="5"/>
       <c r="Q31" s="5"/>
@@ -9020,7 +9205,7 @@
       <c r="T32" s="5"/>
     </row>
     <row r="33" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A33" s="43">
+      <c r="A33" s="41">
         <f>N33</f>
         <v>250</v>
       </c>
@@ -9042,7 +9227,7 @@
         <v>-0.17619232013049979</v>
       </c>
       <c r="G33" s="12"/>
-      <c r="H33" s="46">
+      <c r="H33" s="44">
         <v>1</v>
       </c>
       <c r="J33" s="19">
@@ -9057,7 +9242,7 @@
         <f t="shared" si="13"/>
         <v>1.2415914135117765</v>
       </c>
-      <c r="N33" s="56">
+      <c r="N33" s="54">
         <v>250</v>
       </c>
       <c r="O33" s="27">
@@ -9120,7 +9305,7 @@
       <c r="AN33" s="33"/>
     </row>
     <row r="34" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A34" s="43">
+      <c r="A34" s="41">
         <f t="shared" ref="A34:A36" si="14">N34</f>
         <v>275</v>
       </c>
@@ -9130,7 +9315,7 @@
       <c r="E34" s="12"/>
       <c r="F34" s="12"/>
       <c r="G34" s="12"/>
-      <c r="H34" s="46">
+      <c r="H34" s="44">
         <v>1</v>
       </c>
       <c r="J34" s="19">
@@ -9145,7 +9330,7 @@
         <f t="shared" si="13"/>
         <v>1.2978116854623587</v>
       </c>
-      <c r="N34" s="56">
+      <c r="N34" s="54">
         <v>275</v>
       </c>
       <c r="O34" s="27">
@@ -9208,7 +9393,7 @@
       <c r="AN34" s="33"/>
     </row>
     <row r="35" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A35" s="43">
+      <c r="A35" s="41">
         <f t="shared" si="14"/>
         <v>300</v>
       </c>
@@ -9230,7 +9415,7 @@
         <v>8.7098625265978002E-2</v>
       </c>
       <c r="G35" s="12"/>
-      <c r="H35" s="46">
+      <c r="H35" s="44">
         <v>1</v>
       </c>
       <c r="J35" s="19">
@@ -9245,7 +9430,7 @@
         <f t="shared" si="15"/>
         <v>1.299049117594671</v>
       </c>
-      <c r="N35" s="56">
+      <c r="N35" s="54">
         <v>300</v>
       </c>
       <c r="O35" s="27">
@@ -9308,7 +9493,7 @@
       <c r="AN35" s="33"/>
     </row>
     <row r="36" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A36" s="43">
+      <c r="A36" s="41">
         <f t="shared" si="14"/>
         <v>325</v>
       </c>
@@ -9318,7 +9503,7 @@
       <c r="E36" s="12"/>
       <c r="F36" s="12"/>
       <c r="G36" s="12"/>
-      <c r="H36" s="46">
+      <c r="H36" s="44">
         <v>1</v>
       </c>
       <c r="J36" s="19">
@@ -9333,7 +9518,7 @@
         <f t="shared" si="15"/>
         <v>1.291971968683137</v>
       </c>
-      <c r="N36" s="56">
+      <c r="N36" s="54">
         <v>325</v>
       </c>
       <c r="O36" s="27">
@@ -9403,11 +9588,11 @@
       <c r="E37" s="12"/>
       <c r="F37" s="12"/>
       <c r="G37" s="12"/>
-      <c r="H37" s="46"/>
+      <c r="H37" s="44"/>
       <c r="J37" s="19"/>
       <c r="K37" s="19"/>
       <c r="L37" s="19"/>
-      <c r="N37" s="56"/>
+      <c r="N37" s="54"/>
       <c r="O37" s="27"/>
       <c r="P37" s="27"/>
       <c r="Q37" s="27"/>
@@ -9443,18 +9628,18 @@
       <c r="E38" s="12"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12"/>
-      <c r="H38" s="48"/>
+      <c r="H38" s="46"/>
     </row>
     <row r="39" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="D39" s="67">
+      <c r="D39" s="62">
         <f>AF39+AK39-Q39</f>
         <v>0.6493401796097249</v>
       </c>
-      <c r="E39" s="67">
+      <c r="E39" s="62">
         <f>AG39+AL39-R39</f>
         <v>-0.3530878516527256</v>
       </c>
-      <c r="F39" s="67">
+      <c r="F39" s="62">
         <f t="shared" ref="E39:F40" si="16">AH39+AM39-S39</f>
         <v>-0.55252280147353616</v>
       </c>
@@ -9500,15 +9685,15 @@
       </c>
     </row>
     <row r="40" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="D40" s="67">
+      <c r="D40" s="62">
         <f t="shared" ref="D40" si="20">AF40+AK40-Q40</f>
         <v>0.66114389745121649</v>
       </c>
-      <c r="E40" s="67">
+      <c r="E40" s="62">
         <f t="shared" si="16"/>
         <v>5.3603040621408304E-3</v>
       </c>
-      <c r="F40" s="67">
+      <c r="F40" s="62">
         <f t="shared" si="16"/>
         <v>-6.2339598367251448E-2</v>
       </c>
@@ -9572,33 +9757,33 @@
     <mergeCell ref="Z1:AD1"/>
   </mergeCells>
   <conditionalFormatting sqref="C37:G38 G36">
-    <cfRule type="cellIs" dxfId="6" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J33:L36">
-    <cfRule type="cellIs" dxfId="5" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="greaterThan">
       <formula>1.3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="9" operator="greaterThan">
       <formula>3.19</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36:F36">
-    <cfRule type="cellIs" dxfId="2" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="greaterThan">
       <formula>3.19</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I33:M36">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
       <formula>1.3</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>